<commit_message>
Fix data loading: Auto-load portfolio on startup
- Fixed field mapping issue (camelCase to snake_case)
- Added automatic data loading with delayed initialization
- Fixed portfolio display not showing saved assets on restart
- Added debug logging for data loading process
- Moved save/clear buttons to header row for better UX
- All CRUD operations now working correctly

RESOLVED: Assets save to Excel and load properly on app restart

🚀 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,74 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ETF prova</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fineco</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>22/05/2000</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>22000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>44000</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>22/7/2024</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>3</v>
+      </c>
+      <c r="N2" t="n">
+        <v>27000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>81000</v>
+      </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Prova asset</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Code refactoring: Clean and documented codebase
MAJOR REFACTORING:
- Removed all debug print statements and test functions
- Added comprehensive documentation to all classes and methods
- Cleaned up main.py with clear section comments
- Enhanced models.py with detailed docstrings
- Simplified function names (test_save_asset -> save_new_asset)
- Added header documentation with repository info
- Maintained all functionality while improving code readability

BENEFITS:
- Professional, production-ready code
- Clear documentation for maintenance
- Easier to understand and extend
- Removed temporary debug artifacts

🚀 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,6 +603,82 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MSC World</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fineco</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>sdr4558</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ed38383838</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>22/05/2000</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>234</v>
+      </c>
+      <c r="J3" t="n">
+        <v>23.45</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5487.3</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>23/07/2024</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>278</v>
+      </c>
+      <c r="N3" t="n">
+        <v>25.89</v>
+      </c>
+      <c r="O3" t="n">
+        <v>7197.42</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>ETF di prova</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Major UI improvements: Optimize layout and add advanced portfolio features
- Compress interface spacing: Reduce navbar height from 80px to 65px, optimize padding throughout
- Add dynamic Record/Asset view toggle: Display all historical records vs current assets only
- Implement advanced column filtering: Click headers to filter with popup interfaces
- Add historical record creation: New "Nuovo Record" button for asset evolution tracking
- Enable category-based field management: Auto-enable/disable fields based on asset category
- Add real-time value tracking: "Valore selezionato" shows filtered/selected asset totals
- Improve visual feedback: Stars for active filters, color coding for disabled fields
- Enhanced form validation: NA/0 default values for non-applicable category fields

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16e092a6a9e991bb/GAB_App/GAB_AssetMind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD320DAC9F0481DD04B2998326A75D0F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4240A81A-5772-4836-9435-9EE022620D5D}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_3C25C38B550A53765D41D1F0505ED87656CD1C20" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC67FC8C-F76E-4980-B66F-FFCBFB27879D}"/>
   <bookViews>
-    <workbookView xWindow="15555" yWindow="3488" windowWidth="10125" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="13403" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -97,6 +110,12 @@
     <t>VUSA.MI</t>
   </si>
   <si>
+    <t>2024-11-13</t>
+  </si>
+  <si>
+    <t>2025-05-19</t>
+  </si>
+  <si>
     <t>Autogestito</t>
   </si>
   <si>
@@ -142,7 +161,7 @@
     <t>SWDA.MI</t>
   </si>
   <si>
-    <t>Fineco_+</t>
+    <t>Fineco_Adv+</t>
   </si>
   <si>
     <t>Amundi MSCI Semiconductors ESG Screened UCITS ETF Acc</t>
@@ -154,9 +173,6 @@
     <t>AFF</t>
   </si>
   <si>
-    <t>Advice+</t>
-  </si>
-  <si>
     <t>Invesco EQQQ Nasdaq-100 UCITS ETF Acc EUR</t>
   </si>
   <si>
@@ -176,6 +192,72 @@
   </si>
   <si>
     <t>XETRA</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>FAM MegaTrends L EUR Acc</t>
+  </si>
+  <si>
+    <t>Versamenti periodici</t>
+  </si>
+  <si>
+    <t>Fondi di investimento</t>
+  </si>
+  <si>
+    <t>BGF World Technology Euro E2</t>
+  </si>
+  <si>
+    <t>PIC</t>
+  </si>
+  <si>
+    <t>Pictet-Global Megatrend Selection-R EUR</t>
+  </si>
+  <si>
+    <t>Liquidità</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>2024-11-14</t>
+  </si>
+  <si>
+    <t>2025-05-20</t>
+  </si>
+  <si>
+    <t>Mediobanca_auto</t>
+  </si>
+  <si>
+    <t>IS CR 500 USD-AC EUR</t>
+  </si>
+  <si>
+    <t>IE00B5BMR087</t>
+  </si>
+  <si>
+    <t>Mediobanca_cons</t>
+  </si>
+  <si>
+    <t>NORD1 EU CV BD OP BP</t>
+  </si>
+  <si>
+    <t>LU1915690595</t>
+  </si>
+  <si>
+    <t>SISF STR CR BHC EUR</t>
+  </si>
+  <si>
+    <t>LU1046235815</t>
+  </si>
+  <si>
+    <t>Titoli di stato</t>
+  </si>
+  <si>
+    <t>BTP SHORT TERM 3,60</t>
+  </si>
+  <si>
+    <t>IT0005557084</t>
   </si>
 </sst>
 </file>
@@ -183,7 +265,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,9 +276,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -215,33 +299,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,38 +610,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="8" max="8" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="14" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -585,7 +661,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -600,16 +676,16 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -635,28 +711,30 @@
       <c r="G2">
         <v>3</v>
       </c>
-      <c r="H2" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I2">
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1">
         <v>210</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>33.020000000000003</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K21" si="0">I2*J2</f>
         <v>6934.2000000000007</v>
       </c>
-      <c r="L2" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M2">
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1">
         <v>425</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <v>100.16</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
+        <f t="shared" ref="O2:O21" si="1">M2*N2</f>
         <v>42568</v>
       </c>
       <c r="Q2">
@@ -669,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
@@ -683,36 +761,38 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I3">
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1">
         <v>75</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>102.52</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
+        <f t="shared" si="0"/>
         <v>7689</v>
       </c>
-      <c r="L3" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M3">
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1">
         <v>5</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>102.54</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
+        <f t="shared" si="1"/>
         <v>512.70000000000005</v>
       </c>
       <c r="Q3">
@@ -725,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
@@ -739,39 +819,41 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I4">
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1">
         <v>4200</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>4.8179999999999996</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
         <v>20235.599999999999</v>
       </c>
-      <c r="L4" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M4">
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1">
         <v>4200</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <v>4.835</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
+        <f t="shared" si="1"/>
         <v>20307</v>
       </c>
       <c r="Q4">
@@ -784,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.45">
@@ -798,39 +880,41 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I5">
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1">
         <v>45</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>226.95</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
         <v>10212.75</v>
       </c>
-      <c r="L5" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M5">
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1">
         <v>45</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>230</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
+        <f t="shared" si="1"/>
         <v>10350</v>
       </c>
       <c r="Q5">
@@ -843,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.45">
@@ -857,39 +941,41 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I6">
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1">
         <v>122</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>133.38836000000001</v>
       </c>
-      <c r="K6">
-        <v>16273.379919999999</v>
-      </c>
-      <c r="L6" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M6">
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>16273.379920000001</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="1">
         <v>122</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>139.03</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
+        <f t="shared" si="1"/>
         <v>16961.66</v>
       </c>
       <c r="Q6">
@@ -902,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
@@ -916,39 +1002,41 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I7">
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1">
         <v>400</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>99.86</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
         <v>39944</v>
       </c>
-      <c r="L7" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M7">
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="1">
         <v>450</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <v>100.33</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
+        <f t="shared" si="1"/>
         <v>45148.5</v>
       </c>
       <c r="Q7">
@@ -961,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
@@ -972,42 +1060,44 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I8">
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1">
         <v>180</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>52.79</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
         <v>9502.2000000000007</v>
       </c>
-      <c r="L8" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M8">
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1">
         <v>180</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <v>49.15</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
+        <f t="shared" si="1"/>
         <v>8847</v>
       </c>
       <c r="Q8">
@@ -1018,9 +1108,6 @@
       </c>
       <c r="S8">
         <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
@@ -1031,42 +1118,44 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
         <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I9">
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1">
         <v>40</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>337.94</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
         <v>13517.6</v>
       </c>
-      <c r="L9" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M9">
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1">
         <v>40</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>323.13</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
+        <f t="shared" si="1"/>
         <v>12925.2</v>
       </c>
       <c r="Q9">
@@ -1077,9 +1166,6 @@
       </c>
       <c r="S9">
         <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.45">
@@ -1090,40 +1176,42 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
-      <c r="H10" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I10">
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1">
         <v>230</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>64.680000000000007</v>
       </c>
-      <c r="K10">
-        <v>14876.4</v>
-      </c>
-      <c r="L10" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M10">
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>14876.400000000001</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1">
         <v>230</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <v>64.680000000000007</v>
       </c>
-      <c r="O10">
-        <v>14876.4</v>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>14876.400000000001</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1133,9 +1221,6 @@
       </c>
       <c r="S10">
         <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
@@ -1146,42 +1231,44 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
-      <c r="H11" s="2">
-        <v>45609</v>
-      </c>
-      <c r="I11">
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1">
         <v>190</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>70.64</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
         <v>13421.6</v>
       </c>
-      <c r="L11" s="2">
-        <v>45796</v>
-      </c>
-      <c r="M11">
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="1">
         <v>190</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <v>71.59</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
         <v>13602.1</v>
       </c>
       <c r="Q11">
@@ -1193,11 +1280,541 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11" t="s">
-        <v>44</v>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="1">
+        <v>201.273</v>
+      </c>
+      <c r="J12" s="1">
+        <v>119.3901</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>24030.003597300001</v>
+      </c>
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="1">
+        <v>222.41</v>
+      </c>
+      <c r="N12" s="1">
+        <v>138.06</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>30705.924599999998</v>
+      </c>
+      <c r="P12" s="1">
+        <v>300</v>
+      </c>
+      <c r="T12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1">
+        <v>161.21</v>
+      </c>
+      <c r="J13" s="1">
+        <v>37.2744</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>6009.0060240000003</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="1">
+        <v>161.21</v>
+      </c>
+      <c r="N13" s="1">
+        <v>74.87</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>12069.792700000002</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="1">
+        <v>83.036000000000001</v>
+      </c>
+      <c r="J14" s="1">
+        <v>252.52719999999999</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="0"/>
+        <v>20968.848579199999</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="N14" s="1">
+        <v>313.42</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="1"/>
+        <v>28063.626800000002</v>
+      </c>
+      <c r="P14" s="1">
+        <v>300</v>
+      </c>
+      <c r="T14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2500.06</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="0"/>
+        <v>2500.06</v>
+      </c>
+      <c r="L15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>4152.0200000000004</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="1"/>
+        <v>4152.0200000000004</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>46291.4</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>46291.4</v>
+      </c>
+      <c r="L16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>6361.63</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>6361.63</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="1">
+        <v>20</v>
+      </c>
+      <c r="J17" s="1">
+        <v>549.04100000000005</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>10980.820000000002</v>
+      </c>
+      <c r="L17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="1">
+        <v>20</v>
+      </c>
+      <c r="N17" s="1">
+        <v>562.04999999999995</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>11241</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>549.04100000000005</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="1">
+        <v>40</v>
+      </c>
+      <c r="N18" s="1">
+        <v>562.04999999999995</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>22482</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="1">
+        <v>287.49599999999998</v>
+      </c>
+      <c r="J19" s="1">
+        <v>109.5321</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="0"/>
+        <v>31490.040621599997</v>
+      </c>
+      <c r="L19" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="1">
+        <v>287.49599999999998</v>
+      </c>
+      <c r="N19" s="1">
+        <v>109.5323026407324</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>31490.098879999998</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="1">
+        <v>291.27</v>
+      </c>
+      <c r="J20" s="1">
+        <v>108.1079</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="0"/>
+        <v>31488.588033</v>
+      </c>
+      <c r="L20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="1">
+        <v>291.27</v>
+      </c>
+      <c r="N20" s="1">
+        <v>108.1079003364576</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="1"/>
+        <v>31488.588131000004</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="1">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1">
+        <v>99.518199999999993</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="0"/>
+        <v>2089.8822</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="1">
+        <v>21</v>
+      </c>
+      <c r="N21" s="1">
+        <v>99.518199999999993</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="1"/>
+        <v>2089.8822</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor codebase architecture and remove scipy dependency
- Reorganize project structure with legacy version moved to _Legacy/
- Rename main_refactored.py to main.py as primary version
- Remove scipy dependency and replace with simple numpy interpolation
- Fix window centering functionality for proper startup positioning
- Update GAB_AssetMind.pyw to use refactored version as default
- Add GAB_AssetMind_Legacy.pyw for legacy access
- Maintain Excel data loading functionality (45 records verified)
- Clean up imports and optimize dependencies in requirements.txt

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: GAB <gab@example.com>
Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29301"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16e092a6a9e991bb/GAB_App/GAB_AssetMind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6A5C8FE70A0CD305A7D7EF942A67D2D09A3E09D7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE6F85A9-C889-4CD8-9189-47E0B66FC7D3}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_6A5C8FE709C45829C777E8942AD3E257A07E3D8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E293CC3-E187-4504-99F8-85E682DDA73D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="17380" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Debug_Timeline" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="153">
   <si>
     <t>id</t>
   </si>
@@ -375,22 +378,124 @@
     <t>Via M. D. Orlando 14</t>
   </si>
   <si>
-    <t>Orlando Isx</t>
-  </si>
-  <si>
-    <t>23-05-1997</t>
+    <t>Orlando I_sx</t>
+  </si>
+  <si>
+    <t>16-01-1989</t>
   </si>
   <si>
     <t>04-09-2025</t>
   </si>
   <si>
+    <t>Proprietà NC dal '97</t>
+  </si>
+  <si>
     <t>1989/01/16</t>
   </si>
   <si>
+    <t>Orlando I_dx</t>
+  </si>
+  <si>
+    <t>09-12-1997</t>
+  </si>
+  <si>
+    <t>Proprietà GAB dal '97</t>
+  </si>
+  <si>
+    <t>Orlando G_sx</t>
+  </si>
+  <si>
+    <t>29-12-1997</t>
+  </si>
+  <si>
+    <t>Via Pablo Picasso 2</t>
+  </si>
+  <si>
+    <t>Picasso_GAB</t>
+  </si>
+  <si>
+    <t>08-04-2015</t>
+  </si>
+  <si>
+    <t>Proprietà GAB dal '15</t>
+  </si>
+  <si>
+    <t>Picasso_GA</t>
+  </si>
+  <si>
+    <t>Picasso_RA</t>
+  </si>
+  <si>
+    <t>Picasso_Ale</t>
+  </si>
+  <si>
+    <t>Picasso_Giardino</t>
+  </si>
+  <si>
+    <t>27-05-2015</t>
+  </si>
+  <si>
+    <t>Italiana Assicurazioni</t>
+  </si>
+  <si>
+    <t>polizza 41056498</t>
+  </si>
+  <si>
+    <t>02-11-2020</t>
+  </si>
+  <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>polizza 41056491</t>
+  </si>
+  <si>
+    <t>polizza 41056493</t>
+  </si>
+  <si>
+    <t>polizza 41056495</t>
+  </si>
+  <si>
+    <t>polizza 41056494</t>
+  </si>
+  <si>
+    <t>polizza 41056492</t>
+  </si>
+  <si>
+    <t>CREDEM_GAB</t>
+  </si>
+  <si>
+    <t>2015-05-22</t>
+  </si>
+  <si>
+    <t>2025-09-08</t>
+  </si>
+  <si>
+    <t>CREDEM_Agraba</t>
+  </si>
+  <si>
+    <t>CREDEM_R1</t>
+  </si>
+  <si>
     <t>Data</t>
   </si>
   <si>
     <t>TOTALE</t>
+  </si>
+  <si>
+    <t>1997-12-09</t>
+  </si>
+  <si>
+    <t>1997-12-29</t>
+  </si>
+  <si>
+    <t>2015-04-08</t>
+  </si>
+  <si>
+    <t>2015-05-27</t>
+  </si>
+  <si>
+    <t>2020-11-02</t>
   </si>
 </sst>
 </file>
@@ -400,7 +505,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\€#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,17 +857,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="8" max="8" width="15.73046875" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -871,7 +977,7 @@
         <v>33.020000000000003</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K31" si="0">I2*J2</f>
+        <f t="shared" ref="K2:K48" si="0">I2*J2</f>
         <v>6934.2000000000007</v>
       </c>
       <c r="L2" t="s">
@@ -884,7 +990,7 @@
         <v>100.16</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O31" si="1">M2*N2</f>
+        <f t="shared" ref="O2:O48" si="1">M2*N2</f>
         <v>42568</v>
       </c>
       <c r="P2" t="s">
@@ -903,7 +1009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -964,7 +1070,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1028,7 +1134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1092,7 +1198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1156,7 +1262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1220,7 +1326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1284,7 +1390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1348,7 +1454,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1412,7 +1518,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1476,7 +1582,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1525,7 +1631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1583,7 +1689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1632,7 +1738,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1696,7 +1802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1760,7 +1866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1824,7 +1930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1882,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1940,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1998,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2059,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2138,7 +2244,7 @@
         <v>19.671873000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2214,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2290,7 +2396,7 @@
         <v>104.740071</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2366,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2445,7 +2551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2518,7 +2624,7 @@
         <v>1.0661E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2594,7 +2700,7 @@
         <v>197.044995</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2664,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2734,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2770,11 +2876,11 @@
         <v>1</v>
       </c>
       <c r="N31">
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="O31">
         <f t="shared" si="1"/>
-        <v>200000</v>
+        <v>250000</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2785,11 +2891,14 @@
       <c r="S31">
         <v>0</v>
       </c>
+      <c r="T31" t="s">
+        <v>116</v>
+      </c>
       <c r="U31">
         <v>1</v>
       </c>
       <c r="V31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="W31">
         <v>1</v>
@@ -2798,6 +2907,1190 @@
         <v>100</v>
       </c>
       <c r="Y31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>174000</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>174000</v>
+      </c>
+      <c r="L32" t="s">
+        <v>115</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>250000</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>250000</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32" t="s">
+        <v>120</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32" t="s">
+        <v>114</v>
+      </c>
+      <c r="W32">
+        <v>1</v>
+      </c>
+      <c r="X32" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>174000</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>174000</v>
+      </c>
+      <c r="L33" t="s">
+        <v>115</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>250000</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>250000</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33" t="s">
+        <v>120</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33" t="s">
+        <v>119</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>121</v>
+      </c>
+      <c r="J34">
+        <v>174000</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>200000</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34" t="s">
+        <v>120</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34" t="s">
+        <v>122</v>
+      </c>
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>125</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>234113</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>234113</v>
+      </c>
+      <c r="L35" t="s">
+        <v>115</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>300000</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>300000</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35" t="s">
+        <v>126</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35" t="s">
+        <v>122</v>
+      </c>
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>125</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>234113</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>234113</v>
+      </c>
+      <c r="L36" t="s">
+        <v>115</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>300000</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>300000</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36" t="s">
+        <v>126</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36" t="s">
+        <v>125</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>125</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>234113</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>234113</v>
+      </c>
+      <c r="L37" t="s">
+        <v>115</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>300000</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>300000</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37" t="s">
+        <v>126</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="V37" t="s">
+        <v>125</v>
+      </c>
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>125</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>234113</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>234113</v>
+      </c>
+      <c r="L38" t="s">
+        <v>115</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>300000</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>300000</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38" t="s">
+        <v>126</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="V38" t="s">
+        <v>125</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>290375</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>290375</v>
+      </c>
+      <c r="L39" t="s">
+        <v>115</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>35000</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>35000</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39" t="s">
+        <v>126</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39" t="s">
+        <v>125</v>
+      </c>
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>133</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>94446</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>94446</v>
+      </c>
+      <c r="L40" t="s">
+        <v>135</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>97946.76</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>97946.76</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>2</v>
+      </c>
+      <c r="V40" t="s">
+        <v>70</v>
+      </c>
+      <c r="W40">
+        <v>291.27</v>
+      </c>
+      <c r="X40" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y40">
+        <v>291.27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>39100</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>39100</v>
+      </c>
+      <c r="L41" t="s">
+        <v>135</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>40544.18</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="1"/>
+        <v>40544.18</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="V41" t="s">
+        <v>134</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>61954</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>61954</v>
+      </c>
+      <c r="L42" t="s">
+        <v>135</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>64254.42</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="1"/>
+        <v>64254.42</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="V42" t="s">
+        <v>134</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>134</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>94446</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>94446</v>
+      </c>
+      <c r="L43" t="s">
+        <v>135</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>97946.76</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="1"/>
+        <v>97946.76</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+      <c r="V43" t="s">
+        <v>134</v>
+      </c>
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" t="s">
+        <v>139</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>134</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>61954</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>61954</v>
+      </c>
+      <c r="L44" t="s">
+        <v>135</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>64254.42</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="1"/>
+        <v>64254.42</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+      <c r="V44" t="s">
+        <v>134</v>
+      </c>
+      <c r="W44">
+        <v>1</v>
+      </c>
+      <c r="X44" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>134</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>39100</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>39100</v>
+      </c>
+      <c r="L45" t="s">
+        <v>135</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>40544.18</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="1"/>
+        <v>40544.18</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+      <c r="V45" t="s">
+        <v>134</v>
+      </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
+      <c r="X45" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>142</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
+        <v>143</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>16299.56</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="1"/>
+        <v>16299.56</v>
+      </c>
+      <c r="P46" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+      <c r="V46" t="s">
+        <v>87</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>142</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L47" t="s">
+        <v>143</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>9092.61</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="1"/>
+        <v>9092.61</v>
+      </c>
+      <c r="P47" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+      <c r="V47" t="s">
+        <v>142</v>
+      </c>
+      <c r="W47">
+        <v>1</v>
+      </c>
+      <c r="X47" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>142</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L48" t="s">
+        <v>143</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>39624.480000000003</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="1"/>
+        <v>39624.480000000003</v>
+      </c>
+      <c r="P48" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48" t="s">
+        <v>33</v>
+      </c>
+      <c r="U48">
+        <v>1</v>
+      </c>
+      <c r="V48" t="s">
+        <v>142</v>
+      </c>
+      <c r="W48">
+        <v>1</v>
+      </c>
+      <c r="X48" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y48">
         <v>1</v>
       </c>
     </row>
@@ -2808,23 +4101,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="5" width="20" customWidth="1"/>
+    <col min="2" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -2848,355 +4143,239 @@
         <v>104</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>261000</v>
+      </c>
+      <c r="I2">
+        <v>261000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>435000</v>
+      </c>
+      <c r="I3">
+        <v>435000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>107</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>45000</v>
-      </c>
-      <c r="I2">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>480000</v>
+      </c>
+      <c r="I4">
+        <v>480000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>110</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>72000</v>
-      </c>
-      <c r="I3">
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>152606.72992000001</v>
-      </c>
-      <c r="C4">
-        <v>44998.852176499997</v>
-      </c>
-      <c r="D4">
-        <v>6009.0060240000003</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>72000</v>
-      </c>
-      <c r="I4">
-        <v>275614.58812049998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
       <c r="B5">
-        <v>152606.72992000001</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>44998.852176499997</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>68987.634678600007</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>48791.46</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>2089.8822</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>72000</v>
+        <v>507000</v>
       </c>
       <c r="I5">
-        <v>389474.55897510011</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>507000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B6">
-        <v>152606.72992000001</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>44998.852176499997</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>68987.634678600007</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>48791.46</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2089.8822</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>80000</v>
+        <v>1443452</v>
       </c>
       <c r="I6">
-        <v>397474.55897510011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1443452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B7">
-        <v>169482.71851395999</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>44998.852176499997</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>68987.634678600007</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>48791.46</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>2089.8822</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>80000</v>
+        <v>1443452</v>
       </c>
       <c r="I7">
-        <v>414350.54756906012</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1443452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="B8">
-        <v>180589.85144721999</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>44998.852176499997</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>68987.634678600007</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>48791.46</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>2089.8822</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>80000</v>
+        <v>1733827</v>
       </c>
       <c r="I8">
-        <v>425457.68050232012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>1733827</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>152</v>
       </c>
       <c r="B9">
-        <v>236563.68152722</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>58769.551399999997</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>75048.479710999993</v>
+        <v>391000</v>
       </c>
       <c r="E9">
-        <v>8861.69</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>2089.8822</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>80000</v>
+        <v>1733827</v>
       </c>
       <c r="I9">
-        <v>461333.28483821999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10">
-        <v>236563.68152722</v>
-      </c>
-      <c r="C10">
-        <v>58769.551399999997</v>
-      </c>
-      <c r="D10">
-        <v>75048.479710999993</v>
-      </c>
-      <c r="E10">
-        <v>10513.65</v>
-      </c>
-      <c r="F10">
-        <v>2089.8822</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>80000</v>
-      </c>
-      <c r="I10">
-        <v>462985.24483822001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11">
-        <v>250257.67980325001</v>
-      </c>
-      <c r="C11">
-        <v>58769.551399999997</v>
-      </c>
-      <c r="D11">
-        <v>75048.479710999993</v>
-      </c>
-      <c r="E11">
-        <v>19645.669999999998</v>
-      </c>
-      <c r="F11">
-        <v>2089.8822</v>
-      </c>
-      <c r="G11">
-        <v>1016.34415351</v>
-      </c>
-      <c r="H11">
-        <v>80000</v>
-      </c>
-      <c r="I11">
-        <v>486827.60726775997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12">
-        <v>250257.67980325001</v>
-      </c>
-      <c r="C12">
-        <v>58769.551399999997</v>
-      </c>
-      <c r="D12">
-        <v>75048.479710999993</v>
-      </c>
-      <c r="E12">
-        <v>19645.669999999998</v>
-      </c>
-      <c r="F12">
-        <v>2089.8822</v>
-      </c>
-      <c r="G12">
-        <v>1016.34415351</v>
-      </c>
-      <c r="H12">
-        <v>285000</v>
-      </c>
-      <c r="I12">
-        <v>691827.60726775997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13">
-        <v>257387.76336501</v>
-      </c>
-      <c r="C13">
-        <v>58769.551399999997</v>
-      </c>
-      <c r="D13">
-        <v>75048.479710999993</v>
-      </c>
-      <c r="E13">
-        <v>19645.669999999998</v>
-      </c>
-      <c r="F13">
-        <v>2089.8822</v>
-      </c>
-      <c r="G13">
-        <v>1016.34415351</v>
-      </c>
-      <c r="H13">
-        <v>285000</v>
-      </c>
-      <c r="I13">
-        <v>698957.69082952</v>
+        <v>2124827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance charts and export functionality with comprehensive PDF reporting
Key improvements:
- Enhanced charts UI with filtered data support and timeline visualization
- Comprehensive PDF export with cover page, summaries, and detailed analytics
- Improved asset form with better historical record handling
- Enhanced export capabilities with metadata headers and filter banners
- Updated portfolio data with latest asset information

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Debug_Timeline" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,10 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="€#,##0.00"/>
-  </numFmts>
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,10 +25,6 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -41,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -49,20 +42,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="currency" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y48"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,31 +522,6 @@
           <t>note</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>riskLevel</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>createdAt</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>createdAmount</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>updatedAt</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>updatedAmount</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -579,6 +542,12 @@
           <t>Bitcoin</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
@@ -612,6 +581,7 @@
         <f>M2*N2</f>
         <v/>
       </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
@@ -621,25 +591,7 @@
       <c r="S2" t="n">
         <v>0</v>
       </c>
-      <c r="U2" t="n">
-        <v>5</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="W2" t="n">
-        <v>0.010661</v>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>26/08/2025</t>
-        </is>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.010661</v>
-      </c>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -703,6 +655,9 @@
         <f>M3*N3</f>
         <v/>
       </c>
+      <c r="P3" t="n">
+        <v/>
+      </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
@@ -780,6 +735,9 @@
         <f>M4*N4</f>
         <v/>
       </c>
+      <c r="P4" t="n">
+        <v/>
+      </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
@@ -857,6 +815,9 @@
         <f>M5*N5</f>
         <v/>
       </c>
+      <c r="P5" t="n">
+        <v/>
+      </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
@@ -896,6 +857,9 @@
           <t>IE00B8FHGS14</t>
         </is>
       </c>
+      <c r="F6" t="n">
+        <v/>
+      </c>
       <c r="G6" t="n">
         <v>3</v>
       </c>
@@ -927,6 +891,9 @@
       </c>
       <c r="O6">
         <f>M6*N6</f>
+        <v/>
+      </c>
+      <c r="P6" t="n">
         <v/>
       </c>
       <c r="Q6" t="n">
@@ -968,6 +935,9 @@
           <t>LU1437015735</t>
         </is>
       </c>
+      <c r="F7" t="n">
+        <v/>
+      </c>
       <c r="G7" t="n">
         <v>3</v>
       </c>
@@ -999,6 +969,9 @@
       </c>
       <c r="O7">
         <f>M7*N7</f>
+        <v/>
+      </c>
+      <c r="P7" t="n">
         <v/>
       </c>
       <c r="Q7" t="n">
@@ -1078,6 +1051,9 @@
         <f>M8*N8</f>
         <v/>
       </c>
+      <c r="P8" t="n">
+        <v/>
+      </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
@@ -1155,6 +1131,9 @@
         <f>M9*N9</f>
         <v/>
       </c>
+      <c r="P9" t="n">
+        <v/>
+      </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
@@ -1232,6 +1211,9 @@
         <f>M10*N10</f>
         <v/>
       </c>
+      <c r="P10" t="n">
+        <v/>
+      </c>
       <c r="Q10" t="n">
         <v>0</v>
       </c>
@@ -1309,6 +1291,9 @@
         <f>M11*N11</f>
         <v/>
       </c>
+      <c r="P11" t="n">
+        <v/>
+      </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
@@ -1384,6 +1369,9 @@
       </c>
       <c r="O12">
         <f>M12*N12</f>
+        <v/>
+      </c>
+      <c r="P12" t="n">
         <v/>
       </c>
       <c r="Q12" t="n">
@@ -1425,6 +1413,9 @@
           <t>IE00B5BMR087</t>
         </is>
       </c>
+      <c r="F13" t="n">
+        <v/>
+      </c>
       <c r="G13" t="n">
         <v>3</v>
       </c>
@@ -1456,6 +1447,9 @@
       </c>
       <c r="O13">
         <f>M13*N13</f>
+        <v/>
+      </c>
+      <c r="P13" t="n">
         <v/>
       </c>
       <c r="Q13" t="n">
@@ -1497,6 +1491,9 @@
           <t>IE00B5BMR087</t>
         </is>
       </c>
+      <c r="F14" t="n">
+        <v/>
+      </c>
       <c r="G14" t="n">
         <v>3</v>
       </c>
@@ -1530,6 +1527,9 @@
         <f>M14*N14</f>
         <v/>
       </c>
+      <c r="P14" t="n">
+        <v/>
+      </c>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
@@ -1538,6 +1538,9 @@
       </c>
       <c r="S14" t="n">
         <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -1602,6 +1605,9 @@
         <f>M15*N15</f>
         <v/>
       </c>
+      <c r="P15" t="n">
+        <v/>
+      </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
@@ -1611,24 +1617,8 @@
       <c r="S15" t="n">
         <v>0</v>
       </c>
-      <c r="U15" t="n">
-        <v>1</v>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="Y15" t="n">
-        <v>0</v>
+      <c r="T15" t="n">
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -1693,6 +1683,9 @@
         <f>M16*N16</f>
         <v/>
       </c>
+      <c r="P16" t="n">
+        <v/>
+      </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
@@ -1702,24 +1695,8 @@
       <c r="S16" t="n">
         <v>0</v>
       </c>
-      <c r="U16" t="n">
-        <v>3</v>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>9/4/2025</t>
-        </is>
-      </c>
-      <c r="W16" t="n">
-        <v>104.740071</v>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>26/08/2025</t>
-        </is>
-      </c>
-      <c r="Y16" t="n">
-        <v>104.740071</v>
+      <c r="T16" t="n">
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -1784,6 +1761,9 @@
         <f>M17*N17</f>
         <v/>
       </c>
+      <c r="P17" t="n">
+        <v/>
+      </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
@@ -1797,25 +1777,6 @@
         <is>
           <t>TER 0.07%</t>
         </is>
-      </c>
-      <c r="U17" t="n">
-        <v>3</v>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>28/08/2025</t>
-        </is>
-      </c>
-      <c r="Y17" t="n">
-        <v>19.671873</v>
       </c>
     </row>
     <row r="18">
@@ -1880,6 +1841,9 @@
         <f>M18*N18</f>
         <v/>
       </c>
+      <c r="P18" t="n">
+        <v/>
+      </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
@@ -1889,24 +1853,8 @@
       <c r="S18" t="n">
         <v>0</v>
       </c>
-      <c r="U18" t="n">
-        <v>3</v>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t>26/08/2025</t>
-        </is>
-      </c>
-      <c r="Y18" t="n">
-        <v>0</v>
+      <c r="T18" t="n">
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -1971,6 +1919,9 @@
         <f>M19*N19</f>
         <v/>
       </c>
+      <c r="P19" t="n">
+        <v/>
+      </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
@@ -1980,24 +1931,8 @@
       <c r="S19" t="n">
         <v>0</v>
       </c>
-      <c r="U19" t="n">
-        <v>3</v>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>9/4/2025</t>
-        </is>
-      </c>
-      <c r="W19" t="n">
-        <v>197.044995</v>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>26/08/2025</t>
-        </is>
-      </c>
-      <c r="Y19" t="n">
-        <v>197.044995</v>
+      <c r="T19" t="n">
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -2019,6 +1954,12 @@
           <t>BGF World Technology Euro E2</t>
         </is>
       </c>
+      <c r="E20" t="n">
+        <v/>
+      </c>
+      <c r="F20" t="n">
+        <v/>
+      </c>
       <c r="G20" t="n">
         <v>2</v>
       </c>
@@ -2050,6 +1991,9 @@
       </c>
       <c r="O20">
         <f>M20*N20</f>
+        <v/>
+      </c>
+      <c r="P20" t="n">
         <v/>
       </c>
       <c r="Q20" t="n">
@@ -2086,6 +2030,12 @@
           <t>polizza 41056491</t>
         </is>
       </c>
+      <c r="E21" t="n">
+        <v/>
+      </c>
+      <c r="F21" t="n">
+        <v/>
+      </c>
       <c r="G21" t="n">
         <v>1</v>
       </c>
@@ -2119,6 +2069,9 @@
         <f>M21*N21</f>
         <v/>
       </c>
+      <c r="P21" t="n">
+        <v/>
+      </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
@@ -2128,24 +2081,8 @@
       <c r="S21" t="n">
         <v>0</v>
       </c>
-      <c r="U21" t="n">
-        <v>1</v>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>02-11-2020</t>
-        </is>
-      </c>
-      <c r="W21" t="n">
-        <v>1</v>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="Y21" t="n">
-        <v>1</v>
+      <c r="T21" t="n">
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -2167,6 +2104,12 @@
           <t>polizza 41056492</t>
         </is>
       </c>
+      <c r="E22" t="n">
+        <v/>
+      </c>
+      <c r="F22" t="n">
+        <v/>
+      </c>
       <c r="G22" t="n">
         <v>1</v>
       </c>
@@ -2200,6 +2143,9 @@
         <f>M22*N22</f>
         <v/>
       </c>
+      <c r="P22" t="n">
+        <v/>
+      </c>
       <c r="Q22" t="n">
         <v>0</v>
       </c>
@@ -2209,24 +2155,8 @@
       <c r="S22" t="n">
         <v>0</v>
       </c>
-      <c r="U22" t="n">
-        <v>1</v>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>02-11-2020</t>
-        </is>
-      </c>
-      <c r="W22" t="n">
-        <v>1</v>
-      </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="Y22" t="n">
-        <v>1</v>
+      <c r="T22" t="n">
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -2248,6 +2178,12 @@
           <t>polizza 41056493</t>
         </is>
       </c>
+      <c r="E23" t="n">
+        <v/>
+      </c>
+      <c r="F23" t="n">
+        <v/>
+      </c>
       <c r="G23" t="n">
         <v>1</v>
       </c>
@@ -2281,6 +2217,9 @@
         <f>M23*N23</f>
         <v/>
       </c>
+      <c r="P23" t="n">
+        <v/>
+      </c>
       <c r="Q23" t="n">
         <v>0</v>
       </c>
@@ -2290,24 +2229,8 @@
       <c r="S23" t="n">
         <v>0</v>
       </c>
-      <c r="U23" t="n">
-        <v>1</v>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>02-11-2020</t>
-        </is>
-      </c>
-      <c r="W23" t="n">
-        <v>1</v>
-      </c>
-      <c r="X23" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="Y23" t="n">
-        <v>1</v>
+      <c r="T23" t="n">
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -2329,6 +2252,12 @@
           <t>polizza 41056494</t>
         </is>
       </c>
+      <c r="E24" t="n">
+        <v/>
+      </c>
+      <c r="F24" t="n">
+        <v/>
+      </c>
       <c r="G24" t="n">
         <v>1</v>
       </c>
@@ -2362,6 +2291,9 @@
         <f>M24*N24</f>
         <v/>
       </c>
+      <c r="P24" t="n">
+        <v/>
+      </c>
       <c r="Q24" t="n">
         <v>0</v>
       </c>
@@ -2371,24 +2303,8 @@
       <c r="S24" t="n">
         <v>0</v>
       </c>
-      <c r="U24" t="n">
-        <v>1</v>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>02-11-2020</t>
-        </is>
-      </c>
-      <c r="W24" t="n">
-        <v>1</v>
-      </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="Y24" t="n">
-        <v>1</v>
+      <c r="T24" t="n">
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -2410,6 +2326,12 @@
           <t>polizza 41056495</t>
         </is>
       </c>
+      <c r="E25" t="n">
+        <v/>
+      </c>
+      <c r="F25" t="n">
+        <v/>
+      </c>
       <c r="G25" t="n">
         <v>1</v>
       </c>
@@ -2443,6 +2365,9 @@
         <f>M25*N25</f>
         <v/>
       </c>
+      <c r="P25" t="n">
+        <v/>
+      </c>
       <c r="Q25" t="n">
         <v>0</v>
       </c>
@@ -2452,24 +2377,8 @@
       <c r="S25" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="n">
-        <v>1</v>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>02-11-2020</t>
-        </is>
-      </c>
-      <c r="W25" t="n">
-        <v>1</v>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="Y25" t="n">
-        <v>1</v>
+      <c r="T25" t="n">
+        <v/>
       </c>
     </row>
     <row r="26">
@@ -2491,6 +2400,12 @@
           <t>polizza 41056498</t>
         </is>
       </c>
+      <c r="E26" t="n">
+        <v/>
+      </c>
+      <c r="F26" t="n">
+        <v/>
+      </c>
       <c r="G26" t="n">
         <v>1</v>
       </c>
@@ -2524,6 +2439,9 @@
         <f>M26*N26</f>
         <v/>
       </c>
+      <c r="P26" t="n">
+        <v/>
+      </c>
       <c r="Q26" t="n">
         <v>0</v>
       </c>
@@ -2533,24 +2451,8 @@
       <c r="S26" t="n">
         <v>0</v>
       </c>
-      <c r="U26" t="n">
-        <v>2</v>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>2024-11-14</t>
-        </is>
-      </c>
-      <c r="W26" t="n">
-        <v>291.27</v>
-      </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>2025-05-19</t>
-        </is>
-      </c>
-      <c r="Y26" t="n">
-        <v>291.27</v>
+      <c r="T26" t="n">
+        <v/>
       </c>
     </row>
     <row r="27">
@@ -2577,6 +2479,9 @@
           <t>LU1915690595</t>
         </is>
       </c>
+      <c r="F27" t="n">
+        <v/>
+      </c>
       <c r="G27" t="n">
         <v>2</v>
       </c>
@@ -2610,6 +2515,9 @@
         <f>M27*N27</f>
         <v/>
       </c>
+      <c r="P27" t="n">
+        <v/>
+      </c>
       <c r="Q27" t="n">
         <v>0</v>
       </c>
@@ -2618,6 +2526,9 @@
       </c>
       <c r="S27" t="n">
         <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v/>
       </c>
     </row>
     <row r="28">
@@ -2644,6 +2555,9 @@
           <t>LU1046235815</t>
         </is>
       </c>
+      <c r="F28" t="n">
+        <v/>
+      </c>
       <c r="G28" t="n">
         <v>2</v>
       </c>
@@ -2677,6 +2591,9 @@
         <f>M28*N28</f>
         <v/>
       </c>
+      <c r="P28" t="n">
+        <v/>
+      </c>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
@@ -2685,6 +2602,9 @@
       </c>
       <c r="S28" t="n">
         <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v/>
       </c>
     </row>
     <row r="29">
@@ -2706,6 +2626,12 @@
           <t>Casa Naxos</t>
         </is>
       </c>
+      <c r="E29" t="n">
+        <v/>
+      </c>
+      <c r="F29" t="n">
+        <v/>
+      </c>
       <c r="G29" t="n">
         <v>1</v>
       </c>
@@ -2739,6 +2665,9 @@
         <f>M29*N29</f>
         <v/>
       </c>
+      <c r="P29" t="n">
+        <v/>
+      </c>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
@@ -2748,24 +2677,8 @@
       <c r="S29" t="n">
         <v>0</v>
       </c>
-      <c r="U29" t="n">
-        <v>1</v>
-      </c>
-      <c r="V29" t="inlineStr">
-        <is>
-          <t>2004-05-21</t>
-        </is>
-      </c>
-      <c r="W29" t="n">
-        <v>1</v>
-      </c>
-      <c r="X29" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
-      </c>
-      <c r="Y29" t="n">
-        <v>1</v>
+      <c r="T29" t="n">
+        <v/>
       </c>
     </row>
     <row r="30">
@@ -2787,6 +2700,12 @@
           <t>Garage Naxos</t>
         </is>
       </c>
+      <c r="E30" t="n">
+        <v/>
+      </c>
+      <c r="F30" t="n">
+        <v/>
+      </c>
       <c r="G30" t="n">
         <v>1</v>
       </c>
@@ -2820,6 +2739,9 @@
         <f>M30*N30</f>
         <v/>
       </c>
+      <c r="P30" t="n">
+        <v/>
+      </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
@@ -2829,29 +2751,13 @@
       <c r="S30" t="n">
         <v>0</v>
       </c>
-      <c r="U30" t="n">
-        <v>1</v>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>2006-05-22</t>
-        </is>
-      </c>
-      <c r="W30" t="n">
-        <v>1</v>
-      </c>
-      <c r="X30" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
-      </c>
-      <c r="Y30" t="n">
-        <v>1</v>
+      <c r="T30" t="n">
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2867,6 +2773,12 @@
         <is>
           <t>Orlando G_sx</t>
         </is>
+      </c>
+      <c r="E31" t="n">
+        <v/>
+      </c>
+      <c r="F31" t="n">
+        <v/>
       </c>
       <c r="G31" t="n">
         <v>1</v>
@@ -2888,19 +2800,22 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2008-05-22</t>
         </is>
       </c>
       <c r="M31" t="n">
         <v>1</v>
       </c>
       <c r="N31" t="n">
-        <v>250000</v>
+        <v>180000</v>
       </c>
       <c r="O31">
         <f>M31*N31</f>
         <v/>
       </c>
+      <c r="P31" t="n">
+        <v/>
+      </c>
       <c r="Q31" t="n">
         <v>0</v>
       </c>
@@ -2914,30 +2829,11 @@
         <is>
           <t>Proprietà GAB dal '97</t>
         </is>
-      </c>
-      <c r="U31" t="n">
-        <v>1</v>
-      </c>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>09-12-1997</t>
-        </is>
-      </c>
-      <c r="W31" t="n">
-        <v>1</v>
-      </c>
-      <c r="X31" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y31" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2951,22 +2847,28 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Orlando I_dx</t>
-        </is>
+          <t>Orlando G_sx</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v/>
+      </c>
+      <c r="F32" t="n">
+        <v/>
       </c>
       <c r="G32" t="n">
         <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>1989-01-16</t>
+          <t>1997-01-17</t>
         </is>
       </c>
       <c r="I32" t="n">
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>54590</v>
+        <v>89864</v>
       </c>
       <c r="K32">
         <f>I32*J32</f>
@@ -2974,19 +2876,22 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2008-05-22</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="M32" t="n">
         <v>1</v>
       </c>
       <c r="N32" t="n">
-        <v>180000</v>
+        <v>250000</v>
       </c>
       <c r="O32">
         <f>M32*N32</f>
         <v/>
       </c>
+      <c r="P32" t="n">
+        <v/>
+      </c>
       <c r="Q32" t="n">
         <v>0</v>
       </c>
@@ -3000,30 +2905,11 @@
         <is>
           <t>Proprietà GAB dal '97</t>
         </is>
-      </c>
-      <c r="U32" t="n">
-        <v>1</v>
-      </c>
-      <c r="V32" t="inlineStr">
-        <is>
-          <t>2015-05-22</t>
-        </is>
-      </c>
-      <c r="W32" t="n">
-        <v>1</v>
-      </c>
-      <c r="X32" t="inlineStr">
-        <is>
-          <t>2025-09-08</t>
-        </is>
-      </c>
-      <c r="Y32" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3039,6 +2925,12 @@
         <is>
           <t>Orlando I_dx</t>
         </is>
+      </c>
+      <c r="E33" t="n">
+        <v/>
+      </c>
+      <c r="F33" t="n">
+        <v/>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -3060,19 +2952,22 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2008-05-22</t>
+          <t>1997-12-01</t>
         </is>
       </c>
       <c r="M33" t="n">
         <v>1</v>
       </c>
       <c r="N33" t="n">
-        <v>180000</v>
+        <v>89864</v>
       </c>
       <c r="O33">
         <f>M33*N33</f>
         <v/>
       </c>
+      <c r="P33" t="n">
+        <v/>
+      </c>
       <c r="Q33" t="n">
         <v>0</v>
       </c>
@@ -3090,7 +2985,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3106,6 +3001,12 @@
         <is>
           <t>Orlando I_dx</t>
         </is>
+      </c>
+      <c r="E34" t="n">
+        <v/>
+      </c>
+      <c r="F34" t="n">
+        <v/>
       </c>
       <c r="G34" t="n">
         <v>1</v>
@@ -3127,19 +3028,22 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2025-04-09</t>
+          <t>2008-05-22</t>
         </is>
       </c>
       <c r="M34" t="n">
         <v>1</v>
       </c>
       <c r="N34" t="n">
-        <v>250000</v>
+        <v>180000</v>
       </c>
       <c r="O34">
         <f>M34*N34</f>
         <v/>
       </c>
+      <c r="P34" t="n">
+        <v/>
+      </c>
       <c r="Q34" t="n">
         <v>0</v>
       </c>
@@ -3153,30 +3057,11 @@
         <is>
           <t>Proprietà GAB dal '97</t>
         </is>
-      </c>
-      <c r="U34" t="n">
-        <v>1</v>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>16-01-1989</t>
-        </is>
-      </c>
-      <c r="W34" t="n">
-        <v>1</v>
-      </c>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y34" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3190,8 +3075,14 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Orlando I_sx</t>
-        </is>
+          <t>Orlando I_dx</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v/>
+      </c>
+      <c r="F35" t="n">
+        <v/>
       </c>
       <c r="G35" t="n">
         <v>1</v>
@@ -3213,19 +3104,22 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>1997-01-17</t>
+          <t>2025-04-09</t>
         </is>
       </c>
       <c r="M35" t="n">
         <v>1</v>
       </c>
       <c r="N35" t="n">
-        <v>89864</v>
+        <v>250000</v>
       </c>
       <c r="O35">
         <f>M35*N35</f>
         <v/>
       </c>
+      <c r="P35" t="n">
+        <v/>
+      </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
@@ -3237,32 +3131,13 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>Proprietà NC dal '97</t>
-        </is>
-      </c>
-      <c r="U35" t="n">
-        <v>1</v>
-      </c>
-      <c r="V35" t="inlineStr">
-        <is>
-          <t>1989/01/16</t>
-        </is>
-      </c>
-      <c r="W35" t="n">
-        <v>1</v>
-      </c>
-      <c r="X35" t="inlineStr">
-        <is>
-          <t>2025-09-04</t>
-        </is>
-      </c>
-      <c r="Y35" t="n">
-        <v>1</v>
+          <t>Proprietà GAB dal '97</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3271,27 +3146,33 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Via Pablo Picasso 2</t>
+          <t>Via M. D. Orlando 14</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Picasso_Ale</t>
-        </is>
+          <t>Orlando I_sx</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v/>
+      </c>
+      <c r="F36" t="n">
+        <v/>
       </c>
       <c r="G36" t="n">
         <v>1</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2015-08-04</t>
+          <t>1989-01-16</t>
         </is>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>234113</v>
+        <v>54590</v>
       </c>
       <c r="K36">
         <f>I36*J36</f>
@@ -3299,19 +3180,22 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>1997-01-17</t>
         </is>
       </c>
       <c r="M36" t="n">
         <v>1</v>
       </c>
       <c r="N36" t="n">
-        <v>300000</v>
+        <v>89864</v>
       </c>
       <c r="O36">
         <f>M36*N36</f>
         <v/>
       </c>
+      <c r="P36" t="n">
+        <v/>
+      </c>
       <c r="Q36" t="n">
         <v>0</v>
       </c>
@@ -3323,32 +3207,13 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>Proprietà GAB dal '15</t>
-        </is>
-      </c>
-      <c r="U36" t="n">
-        <v>1</v>
-      </c>
-      <c r="V36" t="inlineStr">
-        <is>
-          <t>08-04-2015</t>
-        </is>
-      </c>
-      <c r="W36" t="n">
-        <v>1</v>
-      </c>
-      <c r="X36" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y36" t="n">
-        <v>1</v>
+          <t>Proprietà NC dal '97</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3357,27 +3222,33 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Via Pablo Picasso 2</t>
+          <t>Via M. D. Orlando 14</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Picasso_GA</t>
-        </is>
+          <t>Orlando I_sx</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v/>
+      </c>
+      <c r="F37" t="n">
+        <v/>
       </c>
       <c r="G37" t="n">
         <v>1</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2015-08-04</t>
+          <t>1989-01-16</t>
         </is>
       </c>
       <c r="I37" t="n">
         <v>1</v>
       </c>
       <c r="J37" t="n">
-        <v>234113</v>
+        <v>54590</v>
       </c>
       <c r="K37">
         <f>I37*J37</f>
@@ -3385,19 +3256,22 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2008-05-22</t>
         </is>
       </c>
       <c r="M37" t="n">
         <v>1</v>
       </c>
       <c r="N37" t="n">
-        <v>300000</v>
+        <v>180000</v>
       </c>
       <c r="O37">
         <f>M37*N37</f>
         <v/>
       </c>
+      <c r="P37" t="n">
+        <v/>
+      </c>
       <c r="Q37" t="n">
         <v>0</v>
       </c>
@@ -3409,32 +3283,13 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>Proprietà GAB dal '15</t>
-        </is>
-      </c>
-      <c r="U37" t="n">
-        <v>1</v>
-      </c>
-      <c r="V37" t="inlineStr">
-        <is>
-          <t>08-04-2015</t>
-        </is>
-      </c>
-      <c r="W37" t="n">
-        <v>1</v>
-      </c>
-      <c r="X37" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y37" t="n">
-        <v>1</v>
+          <t>Proprietà NC dal '97</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3443,27 +3298,33 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Via Pablo Picasso 2</t>
+          <t>Via M. D. Orlando 14</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Picasso_GAB</t>
-        </is>
+          <t>Orlando I_sx</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v/>
+      </c>
+      <c r="F38" t="n">
+        <v/>
       </c>
       <c r="G38" t="n">
         <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2015-08-04</t>
+          <t>1989-01-16</t>
         </is>
       </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>234113</v>
+        <v>54590</v>
       </c>
       <c r="K38">
         <f>I38*J38</f>
@@ -3478,12 +3339,15 @@
         <v>1</v>
       </c>
       <c r="N38" t="n">
-        <v>300000</v>
+        <v>250000</v>
       </c>
       <c r="O38">
         <f>M38*N38</f>
         <v/>
       </c>
+      <c r="P38" t="n">
+        <v/>
+      </c>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
@@ -3495,32 +3359,13 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>Proprietà GAB dal '15</t>
-        </is>
-      </c>
-      <c r="U38" t="n">
-        <v>1</v>
-      </c>
-      <c r="V38" t="inlineStr">
-        <is>
-          <t>29-12-1997</t>
-        </is>
-      </c>
-      <c r="W38" t="n">
-        <v>1</v>
-      </c>
-      <c r="X38" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y38" t="n">
-        <v>1</v>
+          <t>Proprietà NC dal '97</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3534,22 +3379,28 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Picasso_Giardino</t>
-        </is>
+          <t>Picasso_Ale</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v/>
+      </c>
+      <c r="F39" t="n">
+        <v/>
       </c>
       <c r="G39" t="n">
         <v>1</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2015-05-27</t>
+          <t>2015-08-04</t>
         </is>
       </c>
       <c r="I39" t="n">
         <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>290375</v>
+        <v>234113</v>
       </c>
       <c r="K39">
         <f>I39*J39</f>
@@ -3564,12 +3415,15 @@
         <v>1</v>
       </c>
       <c r="N39" t="n">
-        <v>35000</v>
+        <v>300000</v>
       </c>
       <c r="O39">
         <f>M39*N39</f>
         <v/>
       </c>
+      <c r="P39" t="n">
+        <v/>
+      </c>
       <c r="Q39" t="n">
         <v>0</v>
       </c>
@@ -3583,30 +3437,11 @@
         <is>
           <t>Proprietà GAB dal '15</t>
         </is>
-      </c>
-      <c r="U39" t="n">
-        <v>1</v>
-      </c>
-      <c r="V39" t="inlineStr">
-        <is>
-          <t>08-04-2015</t>
-        </is>
-      </c>
-      <c r="W39" t="n">
-        <v>1</v>
-      </c>
-      <c r="X39" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y39" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3620,15 +3455,21 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Picasso_RA</t>
-        </is>
+          <t>Picasso_GA</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v/>
+      </c>
+      <c r="F40" t="n">
+        <v/>
       </c>
       <c r="G40" t="n">
         <v>1</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2015-04-08</t>
+          <t>2015-08-04</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3656,6 +3497,9 @@
         <f>M40*N40</f>
         <v/>
       </c>
+      <c r="P40" t="n">
+        <v/>
+      </c>
       <c r="Q40" t="n">
         <v>0</v>
       </c>
@@ -3669,59 +3513,46 @@
         <is>
           <t>Proprietà GAB dal '15</t>
         </is>
-      </c>
-      <c r="U40" t="n">
-        <v>1</v>
-      </c>
-      <c r="V40" t="inlineStr">
-        <is>
-          <t>08-04-2015</t>
-        </is>
-      </c>
-      <c r="W40" t="n">
-        <v>1</v>
-      </c>
-      <c r="X40" t="inlineStr">
-        <is>
-          <t>04-09-2025</t>
-        </is>
-      </c>
-      <c r="Y40" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Liquidità</t>
+          <t>Immobiliare</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CREDEM_GAB</t>
+          <t>Via Pablo Picasso 2</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>$</t>
-        </is>
+          <t>Picasso_GAB</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v/>
+      </c>
+      <c r="F41" t="n">
+        <v/>
       </c>
       <c r="G41" t="n">
         <v>1</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2015-05-22</t>
+          <t>2015-08-04</t>
         </is>
       </c>
       <c r="I41" t="n">
         <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>234113</v>
       </c>
       <c r="K41">
         <f>I41*J41</f>
@@ -3729,19 +3560,22 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="M41" t="n">
         <v>1</v>
       </c>
       <c r="N41" t="n">
-        <v>16299.56</v>
+        <v>300000</v>
       </c>
       <c r="O41">
         <f>M41*N41</f>
         <v/>
       </c>
+      <c r="P41" t="n">
+        <v/>
+      </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
@@ -3753,61 +3587,48 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>Autogestito</t>
-        </is>
-      </c>
-      <c r="U41" t="n">
-        <v>1</v>
-      </c>
-      <c r="V41" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="W41" t="n">
-        <v>1</v>
-      </c>
-      <c r="X41" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="Y41" t="n">
-        <v>1</v>
+          <t>Proprietà GAB dal '15</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Liquidità</t>
+          <t>Immobiliare</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Fineco_Adv+</t>
+          <t>Via Pablo Picasso 2</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>$</t>
-        </is>
+          <t>Picasso_Giardino</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v/>
+      </c>
+      <c r="F42" t="n">
+        <v/>
       </c>
       <c r="G42" t="n">
         <v>1</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2015-05-27</t>
         </is>
       </c>
       <c r="I42" t="n">
         <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2500.06</v>
+        <v>290375</v>
       </c>
       <c r="K42">
         <f>I42*J42</f>
@@ -3815,19 +3636,22 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2025-05-20</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="M42" t="n">
         <v>1</v>
       </c>
       <c r="N42" t="n">
-        <v>4152.02</v>
+        <v>35000</v>
       </c>
       <c r="O42">
         <f>M42*N42</f>
         <v/>
       </c>
+      <c r="P42" t="n">
+        <v/>
+      </c>
       <c r="Q42" t="n">
         <v>0</v>
       </c>
@@ -3839,42 +3663,48 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>Autogestito</t>
+          <t>Proprietà GAB dal '15</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Liquidità</t>
+          <t>Immobiliare</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Mediobanca_auto</t>
+          <t>Via Pablo Picasso 2</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>$</t>
-        </is>
+          <t>Picasso_RA</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v/>
+      </c>
+      <c r="F43" t="n">
+        <v/>
       </c>
       <c r="G43" t="n">
         <v>1</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2015-04-08</t>
         </is>
       </c>
       <c r="I43" t="n">
         <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>46291.4</v>
+        <v>234113</v>
       </c>
       <c r="K43">
         <f>I43*J43</f>
@@ -3882,19 +3712,22 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="M43" t="n">
         <v>1</v>
       </c>
       <c r="N43" t="n">
-        <v>6361.63</v>
+        <v>300000</v>
       </c>
       <c r="O43">
         <f>M43*N43</f>
         <v/>
       </c>
+      <c r="P43" t="n">
+        <v/>
+      </c>
       <c r="Q43" t="n">
         <v>0</v>
       </c>
@@ -3906,13 +3739,13 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>Autogestito</t>
+          <t>Proprietà GAB dal '15</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3921,7 +3754,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Trade Republic</t>
+          <t>CREDEM_GAB</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3929,12 +3762,18 @@
           <t>$</t>
         </is>
       </c>
+      <c r="E44" t="n">
+        <v/>
+      </c>
+      <c r="F44" t="n">
+        <v/>
+      </c>
       <c r="G44" t="n">
         <v>1</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2015-05-22</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3949,19 +3788,22 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M44" t="n">
         <v>1</v>
       </c>
       <c r="N44" t="n">
-        <v>9132.02</v>
+        <v>16299.56</v>
       </c>
       <c r="O44">
         <f>M44*N44</f>
         <v/>
       </c>
+      <c r="P44" t="n">
+        <v/>
+      </c>
       <c r="Q44" t="n">
         <v>0</v>
       </c>
@@ -3975,34 +3817,15 @@
         <is>
           <t>Autogestito</t>
         </is>
-      </c>
-      <c r="U44" t="n">
-        <v>1</v>
-      </c>
-      <c r="V44" t="inlineStr">
-        <is>
-          <t>9/4/2025</t>
-        </is>
-      </c>
-      <c r="W44" t="n">
-        <v>1</v>
-      </c>
-      <c r="X44" t="inlineStr">
-        <is>
-          <t>26/08/2025</t>
-        </is>
-      </c>
-      <c r="Y44" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>PAC</t>
+          <t>Liquidità</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -4012,22 +3835,28 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>FAM MegaTrends L EUR Acc</t>
-        </is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v/>
+      </c>
+      <c r="F45" t="n">
+        <v/>
       </c>
       <c r="G45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>201.273</v>
+        <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>119.3901</v>
+        <v>2500.06</v>
       </c>
       <c r="K45">
         <f>I45*J45</f>
@@ -4035,60 +3864,75 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>222.41</v>
+        <v>1</v>
       </c>
       <c r="N45" t="n">
-        <v>138.06</v>
+        <v>4152.02</v>
       </c>
       <c r="O45">
         <f>M45*N45</f>
         <v/>
       </c>
       <c r="P45" t="n">
-        <v>300</v>
+        <v/>
+      </c>
+      <c r="Q45" t="n">
+        <v>0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0</v>
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>Versamenti periodici</t>
+          <t>Autogestito</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>PAC</t>
+          <t>Liquidità</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Fineco_Adv+</t>
+          <t>Mediobanca_auto</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Pictet-Global Megatrend Selection-R EUR</t>
-        </is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v/>
+      </c>
+      <c r="F46" t="n">
+        <v/>
       </c>
       <c r="G46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>83.036</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>252.5272</v>
+        <v>46291.4</v>
       </c>
       <c r="K46">
         <f>I46*J46</f>
@@ -4100,61 +3944,71 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>89.54000000000001</v>
+        <v>1</v>
       </c>
       <c r="N46" t="n">
-        <v>313.42</v>
+        <v>6361.63</v>
       </c>
       <c r="O46">
         <f>M46*N46</f>
         <v/>
       </c>
       <c r="P46" t="n">
-        <v>300</v>
+        <v/>
+      </c>
+      <c r="Q46" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0</v>
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>Versamenti periodici</t>
+          <t>Autogestito</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Titoli di stato</t>
+          <t>Liquidità</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mediobanca_cons</t>
+          <t>Trade Republic</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>BTP SHORT TERM 3,60</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>IT0005557084</t>
-        </is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v/>
+      </c>
+      <c r="F47" t="n">
+        <v/>
       </c>
       <c r="G47" t="n">
         <v>1</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2025-08-26</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>99.51819999999999</v>
+        <v>0</v>
       </c>
       <c r="K47">
         <f>I47*J47</f>
@@ -4162,19 +4016,22 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-08-26</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="N47" t="n">
-        <v>99.51819999999999</v>
+        <v>9132.02</v>
       </c>
       <c r="O47">
         <f>M47*N47</f>
         <v/>
       </c>
+      <c r="P47" t="n">
+        <v/>
+      </c>
       <c r="Q47" t="n">
         <v>0</v>
       </c>
@@ -4183,40 +4040,51 @@
       </c>
       <c r="S47" t="n">
         <v>0</v>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>Autogestito</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Immobiliare</t>
+          <t>PAC</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Via M. D. Orlando 14</t>
+          <t>Fineco_Adv+</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Orlando I_sx</t>
-        </is>
+          <t>FAM MegaTrends L EUR Acc</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v/>
+      </c>
+      <c r="F48" t="n">
+        <v/>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>1989-01-16</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>201.273</v>
       </c>
       <c r="J48" t="n">
-        <v>54590</v>
+        <v>119.3901</v>
       </c>
       <c r="K48">
         <f>I48*J48</f>
@@ -4224,853 +4092,187 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-05-19</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>1</v>
+        <v>222.41</v>
       </c>
       <c r="N48" t="n">
-        <v>250000</v>
+        <v>138.06</v>
       </c>
       <c r="O48">
         <f>M48*N48</f>
         <v/>
       </c>
+      <c r="P48" t="n">
+        <v>300</v>
+      </c>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="R48" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="S48" t="n">
-        <v>0</v>
+        <v/>
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>Proprietà NC dal '97</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="17" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Criptovalute</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ETF</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Fondi di investimento</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Immobiliare</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Liquidità</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+          <t>Versamenti periodici</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>13</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>PAC</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Fineco_Adv+</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Pictet-Global Megatrend Selection-R EUR</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v/>
+      </c>
+      <c r="F49" t="n">
+        <v/>
+      </c>
+      <c r="G49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>83.036</v>
+      </c>
+      <c r="J49" t="n">
+        <v>252.5272</v>
+      </c>
+      <c r="K49">
+        <f>I49*J49</f>
+        <v/>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>89.54000000000001</v>
+      </c>
+      <c r="N49" t="n">
+        <v>313.42</v>
+      </c>
+      <c r="O49">
+        <f>M49*N49</f>
+        <v/>
+      </c>
+      <c r="P49" t="n">
+        <v>300</v>
+      </c>
+      <c r="Q49" t="n">
+        <v/>
+      </c>
+      <c r="R49" t="n">
+        <v/>
+      </c>
+      <c r="S49" t="n">
+        <v/>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>Versamenti periodici</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>20</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>Titoli di stato</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>TOTALE</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1989-01-16</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>109180</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>109180</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1997-01-17</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>234318</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>234318</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2004-05-21</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>279318</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>279318</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2006-05-22</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>306318</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>306318</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2008-05-22</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>431728</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>431728</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2015-04-08</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>665841</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>665841</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2015-05-22</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>665841</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>665841</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2015-05-27</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>956216</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>956216</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2015-08-04</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>1658555</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>1658555</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2020-02-11</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>163008</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>1658555</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>1821563</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2020-11-02</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>391000</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1658555</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>2049555</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-11-13</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>152606.72992</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>397009.006024</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1658555</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>2253169.5881205</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mediobanca_cons</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>BTP SHORT TERM 3,60</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>IT0005557084</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v/>
+      </c>
+      <c r="G50" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>2024-11-14</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>174568.36992</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>459987.6346786</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1658555</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>2388991.1989751</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-03-09</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>174568.36992</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>459987.6346786</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>1666555</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>2396991.1989751</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-04-09</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>174568.36992</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>459987.6346786</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>2627127.1989751</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>191444.35851396</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>459987.6346786</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>2644003.18756906</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>202551.49144722</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>459987.6346786</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>2655110.32050232</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="I50" t="n">
+        <v>21</v>
+      </c>
+      <c r="J50" t="n">
+        <v>99.51819999999999</v>
+      </c>
+      <c r="K50">
+        <f>I50*J50</f>
+        <v/>
+      </c>
+      <c r="L50" t="inlineStr">
         <is>
           <t>2025-05-19</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>236563.68152722</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>466048.479711</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>8861.690000000001</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H19" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I19" s="2" t="n">
-        <v>2669024.28483822</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2025-05-20</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>236563.68152722</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>466048.479711</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>10513.65</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H20" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I20" s="2" t="n">
-        <v>2670676.24483822</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>236563.68152722</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>480539.199711</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>10513.65</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H21" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>2685166.96483822</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>1016.34415351</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>250257.67980325</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>480539.199711</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>1896691</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>19645.67</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H22" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I22" s="2" t="n">
-        <v>2709009.327267759</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>1016.34415351</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>250257.67980325</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>480539.199711</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>2101691</v>
-      </c>
-      <c r="F23" s="2" t="n">
-        <v>19645.67</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H23" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I23" s="2" t="n">
-        <v>2914009.327267759</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-09-04</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="n">
-        <v>1016.34415351</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>257387.76336501</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>480539.199711</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F24" s="2" t="n">
-        <v>19645.67</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H24" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I24" s="2" t="n">
-        <v>3089448.41082952</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-09-08</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>1016.34415351</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>257387.76336501</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>480539.199711</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>35945.23</v>
-      </c>
-      <c r="G25" s="2" t="n">
-        <v>58769.5514</v>
-      </c>
-      <c r="H25" s="2" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="I25" s="2" t="n">
-        <v>3105747.970829519</v>
+      <c r="M50" t="n">
+        <v>21</v>
+      </c>
+      <c r="N50" t="n">
+        <v>99.51819999999999</v>
+      </c>
+      <c r="O50">
+        <f>M50*N50</f>
+        <v/>
+      </c>
+      <c r="P50" t="n">
+        <v/>
+      </c>
+      <c r="Q50" t="n">
+        <v>0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0</v>
+      </c>
+      <c r="T50" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add user recommendations section to market update report
Added intelligent recommendations to help users improve future price updates:
- Suggests adding exchange suffixes when TwelveData Pro plan errors occur
- Recommends ticker corrections for invalid symbols
- Alerts about potential delisted tickers
- Warns when price variations are anomalous (>50%) suggesting wrong exchange
- Counts assets missing ticker/ISIN identifiers

Also updated Excel file with corrected tickers:
- ID 67: MVOL -> MVOL.MI (Milan EUR)
- ID 68: A111X9 -> EIMI.MI (Milan EUR)
- ID 63: MLWTE -> (empty - will use BlackRock NAV)

The recommendations appear in the detailed report after errors section,
providing actionable guidance to reduce issues in future updates.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -585,9 +585,6 @@
         <f>M2*N2</f>
         <v/>
       </c>
-      <c r="P2" t="n">
-        <v/>
-      </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
@@ -596,9 +593,6 @@
       </c>
       <c r="S2" t="n">
         <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v/>
       </c>
     </row>
     <row r="3">
@@ -663,9 +657,6 @@
         <f>M3*N3</f>
         <v/>
       </c>
-      <c r="P3" t="n">
-        <v/>
-      </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
@@ -743,9 +734,6 @@
         <f>M4*N4</f>
         <v/>
       </c>
-      <c r="P4" t="n">
-        <v/>
-      </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
@@ -754,9 +742,6 @@
       </c>
       <c r="S4" t="n">
         <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v/>
       </c>
     </row>
     <row r="5">
@@ -821,9 +806,6 @@
         <f>M5*N5</f>
         <v/>
       </c>
-      <c r="P5" t="n">
-        <v/>
-      </c>
       <c r="Q5" t="n">
         <v>0</v>
       </c>
@@ -901,9 +883,6 @@
         <f>M6*N6</f>
         <v/>
       </c>
-      <c r="P6" t="n">
-        <v/>
-      </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
@@ -912,9 +891,6 @@
       </c>
       <c r="S6" t="n">
         <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v/>
       </c>
     </row>
     <row r="7">
@@ -979,9 +955,6 @@
         <f>M7*N7</f>
         <v/>
       </c>
-      <c r="P7" t="n">
-        <v/>
-      </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
@@ -1059,9 +1032,6 @@
         <f>M8*N8</f>
         <v/>
       </c>
-      <c r="P8" t="n">
-        <v/>
-      </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
@@ -1070,9 +1040,6 @@
       </c>
       <c r="S8" t="n">
         <v>0</v>
-      </c>
-      <c r="T8" t="n">
-        <v/>
       </c>
     </row>
     <row r="9">
@@ -1137,9 +1104,6 @@
         <f>M9*N9</f>
         <v/>
       </c>
-      <c r="P9" t="n">
-        <v/>
-      </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
@@ -1181,7 +1145,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MVOL</t>
+          <t>MVOL.MI</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1215,9 +1179,6 @@
       </c>
       <c r="O10">
         <f>M10*N10</f>
-        <v/>
-      </c>
-      <c r="P10" t="n">
         <v/>
       </c>
       <c r="Q10" t="n">
@@ -1297,9 +1258,6 @@
         <f>M11*N11</f>
         <v/>
       </c>
-      <c r="P11" t="n">
-        <v/>
-      </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
@@ -1377,9 +1335,6 @@
         <f>M12*N12</f>
         <v/>
       </c>
-      <c r="P12" t="n">
-        <v/>
-      </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
@@ -1457,9 +1412,6 @@
         <f>M13*N13</f>
         <v/>
       </c>
-      <c r="P13" t="n">
-        <v/>
-      </c>
       <c r="Q13" t="n">
         <v>0</v>
       </c>
@@ -1537,9 +1489,6 @@
         <f>M14*N14</f>
         <v/>
       </c>
-      <c r="P14" t="n">
-        <v/>
-      </c>
       <c r="Q14" t="n">
         <v>0</v>
       </c>
@@ -1617,9 +1566,6 @@
         <f>M15*N15</f>
         <v/>
       </c>
-      <c r="P15" t="n">
-        <v/>
-      </c>
       <c r="Q15" t="n">
         <v>0</v>
       </c>
@@ -1697,9 +1643,6 @@
         <f>M16*N16</f>
         <v/>
       </c>
-      <c r="P16" t="n">
-        <v/>
-      </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
@@ -1777,9 +1720,6 @@
         <f>M17*N17</f>
         <v/>
       </c>
-      <c r="P17" t="n">
-        <v/>
-      </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
@@ -1857,9 +1797,6 @@
         <f>M18*N18</f>
         <v/>
       </c>
-      <c r="P18" t="n">
-        <v/>
-      </c>
       <c r="Q18" t="n">
         <v>0</v>
       </c>
@@ -1937,9 +1874,6 @@
         <f>M19*N19</f>
         <v/>
       </c>
-      <c r="P19" t="n">
-        <v/>
-      </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
@@ -1948,9 +1882,6 @@
       </c>
       <c r="S19" t="n">
         <v>0</v>
-      </c>
-      <c r="T19" t="n">
-        <v/>
       </c>
     </row>
     <row r="20">
@@ -2015,9 +1946,6 @@
         <f>M20*N20</f>
         <v/>
       </c>
-      <c r="P20" t="n">
-        <v/>
-      </c>
       <c r="Q20" t="n">
         <v>0</v>
       </c>
@@ -2095,9 +2023,6 @@
         <f>M21*N21</f>
         <v/>
       </c>
-      <c r="P21" t="n">
-        <v/>
-      </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
@@ -2106,9 +2031,6 @@
       </c>
       <c r="S21" t="n">
         <v>0</v>
-      </c>
-      <c r="T21" t="n">
-        <v/>
       </c>
     </row>
     <row r="22">
@@ -2173,9 +2095,6 @@
         <f>M22*N22</f>
         <v/>
       </c>
-      <c r="P22" t="n">
-        <v/>
-      </c>
       <c r="Q22" t="n">
         <v>0</v>
       </c>
@@ -2253,9 +2172,6 @@
         <f>M23*N23</f>
         <v/>
       </c>
-      <c r="P23" t="n">
-        <v/>
-      </c>
       <c r="Q23" t="n">
         <v>0</v>
       </c>
@@ -2333,9 +2249,6 @@
         <f>M24*N24</f>
         <v/>
       </c>
-      <c r="P24" t="n">
-        <v/>
-      </c>
       <c r="Q24" t="n">
         <v>0</v>
       </c>
@@ -2377,7 +2290,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>A111X9</t>
+          <t>EIMI.MI</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2411,9 +2324,6 @@
       </c>
       <c r="O25">
         <f>M25*N25</f>
-        <v/>
-      </c>
-      <c r="P25" t="n">
         <v/>
       </c>
       <c r="Q25" t="n">
@@ -2493,9 +2403,6 @@
         <f>M26*N26</f>
         <v/>
       </c>
-      <c r="P26" t="n">
-        <v/>
-      </c>
       <c r="Q26" t="n">
         <v>0</v>
       </c>
@@ -2504,9 +2411,6 @@
       </c>
       <c r="S26" t="n">
         <v>0</v>
-      </c>
-      <c r="T26" t="n">
-        <v/>
       </c>
     </row>
     <row r="27">
@@ -2571,9 +2475,6 @@
         <f>M27*N27</f>
         <v/>
       </c>
-      <c r="P27" t="n">
-        <v/>
-      </c>
       <c r="Q27" t="n">
         <v>0</v>
       </c>
@@ -2651,9 +2552,6 @@
         <f>M28*N28</f>
         <v/>
       </c>
-      <c r="P28" t="n">
-        <v/>
-      </c>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
@@ -2731,9 +2629,6 @@
         <f>M29*N29</f>
         <v/>
       </c>
-      <c r="P29" t="n">
-        <v/>
-      </c>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
@@ -2765,7 +2660,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MSCI World USD (Acc)</t>
+          <t>Core MSCI World USD (Acc)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2775,7 +2670,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>MWRD</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -2809,9 +2704,6 @@
       </c>
       <c r="O30">
         <f>M30*N30</f>
-        <v/>
-      </c>
-      <c r="P30" t="n">
         <v/>
       </c>
       <c r="Q30" t="n">
@@ -2845,7 +2737,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>MSCI World USD (Acc)</t>
+          <t>Core MSCI World USD (Acc)</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2855,7 +2747,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>MWRD</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -2889,9 +2781,6 @@
       </c>
       <c r="O31">
         <f>M31*N31</f>
-        <v/>
-      </c>
-      <c r="P31" t="n">
         <v/>
       </c>
       <c r="Q31" t="n">
@@ -2930,12 +2819,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>IE000BI8OT95</t>
+          <t>IE00B3WJKG14</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>QDVE.DE</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -2971,9 +2860,6 @@
         <f>M32*N32</f>
         <v/>
       </c>
-      <c r="P32" t="n">
-        <v/>
-      </c>
       <c r="Q32" t="n">
         <v>0</v>
       </c>
@@ -2982,9 +2868,6 @@
       </c>
       <c r="S32" t="n">
         <v>0</v>
-      </c>
-      <c r="T32" t="n">
-        <v/>
       </c>
     </row>
     <row r="33">
@@ -3008,12 +2891,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>IE000BI8OT95</t>
+          <t>IE00B3WJKG14</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>QDVE.DE</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -3047,9 +2930,6 @@
       </c>
       <c r="O33">
         <f>M33*N33</f>
-        <v/>
-      </c>
-      <c r="P33" t="n">
         <v/>
       </c>
       <c r="Q33" t="n">
@@ -3129,9 +3009,6 @@
         <f>M34*N34</f>
         <v/>
       </c>
-      <c r="P34" t="n">
-        <v/>
-      </c>
       <c r="Q34" t="n">
         <v>0</v>
       </c>
@@ -3171,11 +3048,7 @@
           <t>LU0171310955</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>MLWTE</t>
-        </is>
-      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
         <v>4</v>
       </c>
@@ -3207,9 +3080,6 @@
       </c>
       <c r="O35">
         <f>M35*N35</f>
-        <v/>
-      </c>
-      <c r="P35" t="n">
         <v/>
       </c>
       <c r="Q35" t="n">
@@ -3289,9 +3159,6 @@
         <f>M36*N36</f>
         <v/>
       </c>
-      <c r="P36" t="n">
-        <v/>
-      </c>
       <c r="Q36" t="n">
         <v>0</v>
       </c>
@@ -3369,9 +3236,6 @@
         <f>M37*N37</f>
         <v/>
       </c>
-      <c r="P37" t="n">
-        <v/>
-      </c>
       <c r="Q37" t="n">
         <v>0</v>
       </c>
@@ -3449,9 +3313,6 @@
         <f>M38*N38</f>
         <v/>
       </c>
-      <c r="P38" t="n">
-        <v/>
-      </c>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
@@ -3529,9 +3390,6 @@
         <f>M39*N39</f>
         <v/>
       </c>
-      <c r="P39" t="n">
-        <v/>
-      </c>
       <c r="Q39" t="n">
         <v>0</v>
       </c>
@@ -3566,12 +3424,6 @@
           <t>Casa Naxos</t>
         </is>
       </c>
-      <c r="E40" t="n">
-        <v/>
-      </c>
-      <c r="F40" t="n">
-        <v/>
-      </c>
       <c r="G40" t="n">
         <v>1</v>
       </c>
@@ -3605,9 +3457,6 @@
         <f>M40*N40</f>
         <v/>
       </c>
-      <c r="P40" t="n">
-        <v/>
-      </c>
       <c r="Q40" t="n">
         <v>0</v>
       </c>
@@ -3616,9 +3465,6 @@
       </c>
       <c r="S40" t="n">
         <v>0</v>
-      </c>
-      <c r="T40" t="n">
-        <v/>
       </c>
     </row>
     <row r="41">
@@ -3640,12 +3486,6 @@
           <t>Garage Naxos</t>
         </is>
       </c>
-      <c r="E41" t="n">
-        <v/>
-      </c>
-      <c r="F41" t="n">
-        <v/>
-      </c>
       <c r="G41" t="n">
         <v>1</v>
       </c>
@@ -3679,9 +3519,6 @@
         <f>M41*N41</f>
         <v/>
       </c>
-      <c r="P41" t="n">
-        <v/>
-      </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
@@ -3690,9 +3527,6 @@
       </c>
       <c r="S41" t="n">
         <v>0</v>
-      </c>
-      <c r="T41" t="n">
-        <v/>
       </c>
     </row>
     <row r="42">
@@ -3714,12 +3548,6 @@
           <t>Orlando G_sx</t>
         </is>
       </c>
-      <c r="E42" t="n">
-        <v/>
-      </c>
-      <c r="F42" t="n">
-        <v/>
-      </c>
       <c r="G42" t="n">
         <v>1</v>
       </c>
@@ -3753,9 +3581,6 @@
         <f>M42*N42</f>
         <v/>
       </c>
-      <c r="P42" t="n">
-        <v/>
-      </c>
       <c r="Q42" t="n">
         <v>0</v>
       </c>
@@ -3764,9 +3589,6 @@
       </c>
       <c r="S42" t="n">
         <v>0</v>
-      </c>
-      <c r="T42" t="n">
-        <v/>
       </c>
     </row>
     <row r="43">
@@ -3788,12 +3610,6 @@
           <t>Orlando G_sx</t>
         </is>
       </c>
-      <c r="E43" t="n">
-        <v/>
-      </c>
-      <c r="F43" t="n">
-        <v/>
-      </c>
       <c r="G43" t="n">
         <v>1</v>
       </c>
@@ -3827,9 +3643,6 @@
         <f>M43*N43</f>
         <v/>
       </c>
-      <c r="P43" t="n">
-        <v/>
-      </c>
       <c r="Q43" t="n">
         <v>0</v>
       </c>
@@ -3838,9 +3651,6 @@
       </c>
       <c r="S43" t="n">
         <v>0</v>
-      </c>
-      <c r="T43" t="n">
-        <v/>
       </c>
     </row>
     <row r="44">
@@ -3862,12 +3672,6 @@
           <t>Orlando I_dx</t>
         </is>
       </c>
-      <c r="E44" t="n">
-        <v/>
-      </c>
-      <c r="F44" t="n">
-        <v/>
-      </c>
       <c r="G44" t="n">
         <v>1</v>
       </c>
@@ -3901,9 +3705,6 @@
         <f>M44*N44</f>
         <v/>
       </c>
-      <c r="P44" t="n">
-        <v/>
-      </c>
       <c r="Q44" t="n">
         <v>0</v>
       </c>
@@ -3912,9 +3713,6 @@
       </c>
       <c r="S44" t="n">
         <v>0</v>
-      </c>
-      <c r="T44" t="n">
-        <v/>
       </c>
     </row>
     <row r="45">
@@ -3936,12 +3734,6 @@
           <t>Orlando I_dx</t>
         </is>
       </c>
-      <c r="E45" t="n">
-        <v/>
-      </c>
-      <c r="F45" t="n">
-        <v/>
-      </c>
       <c r="G45" t="n">
         <v>1</v>
       </c>
@@ -3975,9 +3767,6 @@
         <f>M45*N45</f>
         <v/>
       </c>
-      <c r="P45" t="n">
-        <v/>
-      </c>
       <c r="Q45" t="n">
         <v>0</v>
       </c>
@@ -3986,9 +3775,6 @@
       </c>
       <c r="S45" t="n">
         <v>0</v>
-      </c>
-      <c r="T45" t="n">
-        <v/>
       </c>
     </row>
     <row r="46">
@@ -4010,12 +3796,6 @@
           <t>Orlando I_dx</t>
         </is>
       </c>
-      <c r="E46" t="n">
-        <v/>
-      </c>
-      <c r="F46" t="n">
-        <v/>
-      </c>
       <c r="G46" t="n">
         <v>1</v>
       </c>
@@ -4049,9 +3829,6 @@
         <f>M46*N46</f>
         <v/>
       </c>
-      <c r="P46" t="n">
-        <v/>
-      </c>
       <c r="Q46" t="n">
         <v>0</v>
       </c>
@@ -4060,9 +3837,6 @@
       </c>
       <c r="S46" t="n">
         <v>0</v>
-      </c>
-      <c r="T46" t="n">
-        <v/>
       </c>
     </row>
     <row r="47">
@@ -4084,12 +3858,6 @@
           <t>Orlando I_sx</t>
         </is>
       </c>
-      <c r="E47" t="n">
-        <v/>
-      </c>
-      <c r="F47" t="n">
-        <v/>
-      </c>
       <c r="G47" t="n">
         <v>1</v>
       </c>
@@ -4123,9 +3891,6 @@
         <f>M47*N47</f>
         <v/>
       </c>
-      <c r="P47" t="n">
-        <v/>
-      </c>
       <c r="Q47" t="n">
         <v>0</v>
       </c>
@@ -4134,9 +3899,6 @@
       </c>
       <c r="S47" t="n">
         <v>0</v>
-      </c>
-      <c r="T47" t="n">
-        <v/>
       </c>
     </row>
     <row r="48">
@@ -4158,12 +3920,6 @@
           <t>Orlando I_sx</t>
         </is>
       </c>
-      <c r="E48" t="n">
-        <v/>
-      </c>
-      <c r="F48" t="n">
-        <v/>
-      </c>
       <c r="G48" t="n">
         <v>1</v>
       </c>
@@ -4197,9 +3953,6 @@
         <f>M48*N48</f>
         <v/>
       </c>
-      <c r="P48" t="n">
-        <v/>
-      </c>
       <c r="Q48" t="n">
         <v>0</v>
       </c>
@@ -4208,9 +3961,6 @@
       </c>
       <c r="S48" t="n">
         <v>0</v>
-      </c>
-      <c r="T48" t="n">
-        <v/>
       </c>
     </row>
     <row r="49">
@@ -4232,12 +3982,6 @@
           <t>Orlando I_sx</t>
         </is>
       </c>
-      <c r="E49" t="n">
-        <v/>
-      </c>
-      <c r="F49" t="n">
-        <v/>
-      </c>
       <c r="G49" t="n">
         <v>1</v>
       </c>
@@ -4271,9 +4015,6 @@
         <f>M49*N49</f>
         <v/>
       </c>
-      <c r="P49" t="n">
-        <v/>
-      </c>
       <c r="Q49" t="n">
         <v>0</v>
       </c>
@@ -4282,9 +4023,6 @@
       </c>
       <c r="S49" t="n">
         <v>0</v>
-      </c>
-      <c r="T49" t="n">
-        <v/>
       </c>
     </row>
     <row r="50">
@@ -4306,12 +4044,6 @@
           <t>Picasso_Ale</t>
         </is>
       </c>
-      <c r="E50" t="n">
-        <v/>
-      </c>
-      <c r="F50" t="n">
-        <v/>
-      </c>
       <c r="G50" t="n">
         <v>1</v>
       </c>
@@ -4345,9 +4077,6 @@
         <f>M50*N50</f>
         <v/>
       </c>
-      <c r="P50" t="n">
-        <v/>
-      </c>
       <c r="Q50" t="n">
         <v>0</v>
       </c>
@@ -4356,9 +4085,6 @@
       </c>
       <c r="S50" t="n">
         <v>0</v>
-      </c>
-      <c r="T50" t="n">
-        <v/>
       </c>
     </row>
     <row r="51">
@@ -4380,12 +4106,6 @@
           <t>Picasso_GA</t>
         </is>
       </c>
-      <c r="E51" t="n">
-        <v/>
-      </c>
-      <c r="F51" t="n">
-        <v/>
-      </c>
       <c r="G51" t="n">
         <v>1</v>
       </c>
@@ -4419,9 +4139,6 @@
         <f>M51*N51</f>
         <v/>
       </c>
-      <c r="P51" t="n">
-        <v/>
-      </c>
       <c r="Q51" t="n">
         <v>0</v>
       </c>
@@ -4430,9 +4147,6 @@
       </c>
       <c r="S51" t="n">
         <v>0</v>
-      </c>
-      <c r="T51" t="n">
-        <v/>
       </c>
     </row>
     <row r="52">
@@ -4454,12 +4168,6 @@
           <t>Picasso_GAB</t>
         </is>
       </c>
-      <c r="E52" t="n">
-        <v/>
-      </c>
-      <c r="F52" t="n">
-        <v/>
-      </c>
       <c r="G52" t="n">
         <v>1</v>
       </c>
@@ -4493,9 +4201,6 @@
         <f>M52*N52</f>
         <v/>
       </c>
-      <c r="P52" t="n">
-        <v/>
-      </c>
       <c r="Q52" t="n">
         <v>0</v>
       </c>
@@ -4504,9 +4209,6 @@
       </c>
       <c r="S52" t="n">
         <v>0</v>
-      </c>
-      <c r="T52" t="n">
-        <v/>
       </c>
     </row>
     <row r="53">
@@ -4528,12 +4230,6 @@
           <t>Picasso_Giardino</t>
         </is>
       </c>
-      <c r="E53" t="n">
-        <v/>
-      </c>
-      <c r="F53" t="n">
-        <v/>
-      </c>
       <c r="G53" t="n">
         <v>1</v>
       </c>
@@ -4567,9 +4263,6 @@
         <f>M53*N53</f>
         <v/>
       </c>
-      <c r="P53" t="n">
-        <v/>
-      </c>
       <c r="Q53" t="n">
         <v>0</v>
       </c>
@@ -4578,9 +4271,6 @@
       </c>
       <c r="S53" t="n">
         <v>0</v>
-      </c>
-      <c r="T53" t="n">
-        <v/>
       </c>
     </row>
     <row r="54">
@@ -4602,12 +4292,6 @@
           <t>Picasso_RA</t>
         </is>
       </c>
-      <c r="E54" t="n">
-        <v/>
-      </c>
-      <c r="F54" t="n">
-        <v/>
-      </c>
       <c r="G54" t="n">
         <v>1</v>
       </c>
@@ -4641,9 +4325,6 @@
         <f>M54*N54</f>
         <v/>
       </c>
-      <c r="P54" t="n">
-        <v/>
-      </c>
       <c r="Q54" t="n">
         <v>0</v>
       </c>
@@ -4652,9 +4333,6 @@
       </c>
       <c r="S54" t="n">
         <v>0</v>
-      </c>
-      <c r="T54" t="n">
-        <v/>
       </c>
     </row>
     <row r="55">
@@ -4676,12 +4354,6 @@
           <t>$</t>
         </is>
       </c>
-      <c r="E55" t="n">
-        <v/>
-      </c>
-      <c r="F55" t="n">
-        <v/>
-      </c>
       <c r="G55" t="n">
         <v>1</v>
       </c>
@@ -4713,9 +4385,6 @@
       </c>
       <c r="O55">
         <f>M55*N55</f>
-        <v/>
-      </c>
-      <c r="P55" t="n">
         <v/>
       </c>
       <c r="Q55" t="n">
@@ -4752,12 +4421,6 @@
           <t>$</t>
         </is>
       </c>
-      <c r="E56" t="n">
-        <v/>
-      </c>
-      <c r="F56" t="n">
-        <v/>
-      </c>
       <c r="G56" t="n">
         <v>1</v>
       </c>
@@ -4789,9 +4452,6 @@
       </c>
       <c r="O56">
         <f>M56*N56</f>
-        <v/>
-      </c>
-      <c r="P56" t="n">
         <v/>
       </c>
       <c r="Q56" t="n">
@@ -4828,12 +4488,6 @@
           <t>$</t>
         </is>
       </c>
-      <c r="E57" t="n">
-        <v/>
-      </c>
-      <c r="F57" t="n">
-        <v/>
-      </c>
       <c r="G57" t="n">
         <v>1</v>
       </c>
@@ -4865,9 +4519,6 @@
       </c>
       <c r="O57">
         <f>M57*N57</f>
-        <v/>
-      </c>
-      <c r="P57" t="n">
         <v/>
       </c>
       <c r="Q57" t="n">
@@ -4904,12 +4555,6 @@
           <t>$</t>
         </is>
       </c>
-      <c r="E58" t="n">
-        <v/>
-      </c>
-      <c r="F58" t="n">
-        <v/>
-      </c>
       <c r="G58" t="n">
         <v>1</v>
       </c>
@@ -4943,9 +4588,6 @@
         <f>M58*N58</f>
         <v/>
       </c>
-      <c r="P58" t="n">
-        <v/>
-      </c>
       <c r="Q58" t="n">
         <v>0</v>
       </c>
@@ -4954,9 +4596,6 @@
       </c>
       <c r="S58" t="n">
         <v>0</v>
-      </c>
-      <c r="T58" t="n">
-        <v/>
       </c>
     </row>
     <row r="59">
@@ -4978,12 +4617,6 @@
           <t>polizza 41056491</t>
         </is>
       </c>
-      <c r="E59" t="n">
-        <v/>
-      </c>
-      <c r="F59" t="n">
-        <v/>
-      </c>
       <c r="G59" t="n">
         <v>1</v>
       </c>
@@ -5017,9 +4650,6 @@
         <f>M59*N59</f>
         <v/>
       </c>
-      <c r="P59" t="n">
-        <v/>
-      </c>
       <c r="Q59" t="n">
         <v>0</v>
       </c>
@@ -5028,9 +4658,6 @@
       </c>
       <c r="S59" t="n">
         <v>0</v>
-      </c>
-      <c r="T59" t="n">
-        <v/>
       </c>
     </row>
     <row r="60">
@@ -5052,12 +4679,6 @@
           <t>polizza 41056492</t>
         </is>
       </c>
-      <c r="E60" t="n">
-        <v/>
-      </c>
-      <c r="F60" t="n">
-        <v/>
-      </c>
       <c r="G60" t="n">
         <v>1</v>
       </c>
@@ -5091,9 +4712,6 @@
         <f>M60*N60</f>
         <v/>
       </c>
-      <c r="P60" t="n">
-        <v/>
-      </c>
       <c r="Q60" t="n">
         <v>0</v>
       </c>
@@ -5102,9 +4720,6 @@
       </c>
       <c r="S60" t="n">
         <v>0</v>
-      </c>
-      <c r="T60" t="n">
-        <v/>
       </c>
     </row>
     <row r="61">
@@ -5126,12 +4741,6 @@
           <t>polizza 41056493</t>
         </is>
       </c>
-      <c r="E61" t="n">
-        <v/>
-      </c>
-      <c r="F61" t="n">
-        <v/>
-      </c>
       <c r="G61" t="n">
         <v>1</v>
       </c>
@@ -5165,9 +4774,6 @@
         <f>M61*N61</f>
         <v/>
       </c>
-      <c r="P61" t="n">
-        <v/>
-      </c>
       <c r="Q61" t="n">
         <v>0</v>
       </c>
@@ -5176,9 +4782,6 @@
       </c>
       <c r="S61" t="n">
         <v>0</v>
-      </c>
-      <c r="T61" t="n">
-        <v/>
       </c>
     </row>
     <row r="62">
@@ -5200,12 +4803,6 @@
           <t>polizza 41056494</t>
         </is>
       </c>
-      <c r="E62" t="n">
-        <v/>
-      </c>
-      <c r="F62" t="n">
-        <v/>
-      </c>
       <c r="G62" t="n">
         <v>1</v>
       </c>
@@ -5239,9 +4836,6 @@
         <f>M62*N62</f>
         <v/>
       </c>
-      <c r="P62" t="n">
-        <v/>
-      </c>
       <c r="Q62" t="n">
         <v>0</v>
       </c>
@@ -5250,9 +4844,6 @@
       </c>
       <c r="S62" t="n">
         <v>0</v>
-      </c>
-      <c r="T62" t="n">
-        <v/>
       </c>
     </row>
     <row r="63">
@@ -5274,12 +4865,6 @@
           <t>polizza 41056495</t>
         </is>
       </c>
-      <c r="E63" t="n">
-        <v/>
-      </c>
-      <c r="F63" t="n">
-        <v/>
-      </c>
       <c r="G63" t="n">
         <v>1</v>
       </c>
@@ -5313,9 +4898,6 @@
         <f>M63*N63</f>
         <v/>
       </c>
-      <c r="P63" t="n">
-        <v/>
-      </c>
       <c r="Q63" t="n">
         <v>0</v>
       </c>
@@ -5324,9 +4906,6 @@
       </c>
       <c r="S63" t="n">
         <v>0</v>
-      </c>
-      <c r="T63" t="n">
-        <v/>
       </c>
     </row>
     <row r="64">
@@ -5348,12 +4927,6 @@
           <t>polizza 41056498</t>
         </is>
       </c>
-      <c r="E64" t="n">
-        <v/>
-      </c>
-      <c r="F64" t="n">
-        <v/>
-      </c>
       <c r="G64" t="n">
         <v>1</v>
       </c>
@@ -5387,9 +4960,6 @@
         <f>M64*N64</f>
         <v/>
       </c>
-      <c r="P64" t="n">
-        <v/>
-      </c>
       <c r="Q64" t="n">
         <v>0</v>
       </c>
@@ -5398,9 +4968,6 @@
       </c>
       <c r="S64" t="n">
         <v>0</v>
-      </c>
-      <c r="T64" t="n">
-        <v/>
       </c>
     </row>
     <row r="65">
@@ -5422,12 +4989,6 @@
           <t>FAM MegaTrends L EUR Acc</t>
         </is>
       </c>
-      <c r="E65" t="n">
-        <v/>
-      </c>
-      <c r="F65" t="n">
-        <v/>
-      </c>
       <c r="G65" t="n">
         <v>2</v>
       </c>
@@ -5463,15 +5024,6 @@
       </c>
       <c r="P65" t="n">
         <v>300</v>
-      </c>
-      <c r="Q65" t="n">
-        <v/>
-      </c>
-      <c r="R65" t="n">
-        <v/>
-      </c>
-      <c r="S65" t="n">
-        <v/>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -5498,12 +5050,6 @@
           <t>Pictet-Global Megatrend Selection-R EUR</t>
         </is>
       </c>
-      <c r="E66" t="n">
-        <v/>
-      </c>
-      <c r="F66" t="n">
-        <v/>
-      </c>
       <c r="G66" t="n">
         <v>2</v>
       </c>
@@ -5539,15 +5085,6 @@
       </c>
       <c r="P66" t="n">
         <v>300</v>
-      </c>
-      <c r="Q66" t="n">
-        <v/>
-      </c>
-      <c r="R66" t="n">
-        <v/>
-      </c>
-      <c r="S66" t="n">
-        <v/>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -5579,9 +5116,6 @@
           <t>IT0005557084</t>
         </is>
       </c>
-      <c r="F67" t="n">
-        <v/>
-      </c>
       <c r="G67" t="n">
         <v>1</v>
       </c>
@@ -5613,9 +5147,6 @@
       </c>
       <c r="O67">
         <f>M67*N67</f>
-        <v/>
-      </c>
-      <c r="P67" t="n">
         <v/>
       </c>
       <c r="Q67" t="n">
@@ -5657,9 +5188,6 @@
           <t>IT0005557084</t>
         </is>
       </c>
-      <c r="F68" t="n">
-        <v/>
-      </c>
       <c r="G68" t="n">
         <v>1</v>
       </c>
@@ -5691,9 +5219,6 @@
       </c>
       <c r="O68">
         <f>M68*N68</f>
-        <v/>
-      </c>
-      <c r="P68" t="n">
         <v/>
       </c>
       <c r="Q68" t="n">
@@ -5767,13 +5292,10 @@
         <v>0.010661</v>
       </c>
       <c r="N69" t="n">
-        <v>104200.27</v>
+        <v>104018.22</v>
       </c>
       <c r="O69">
         <f>M69*N69</f>
-        <v/>
-      </c>
-      <c r="P69" t="n">
         <v/>
       </c>
       <c r="Q69" t="n">
@@ -5847,15 +5369,12 @@
         <v>180</v>
       </c>
       <c r="N70" t="n">
-        <v>78.19000200000001</v>
+        <v>66.68000000000001</v>
       </c>
       <c r="O70">
         <f>M70*N70</f>
         <v/>
       </c>
-      <c r="P70" t="n">
-        <v/>
-      </c>
       <c r="Q70" t="n">
         <v>0</v>
       </c>
@@ -5867,7 +5386,7 @@
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind | PRICE ALERT</t>
+          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -5927,15 +5446,12 @@
         <v>40</v>
       </c>
       <c r="N71" t="n">
-        <v>141.660004</v>
+        <v>362.540009</v>
       </c>
       <c r="O71">
         <f>M71*N71</f>
         <v/>
       </c>
-      <c r="P71" t="n">
-        <v/>
-      </c>
       <c r="Q71" t="n">
         <v>0</v>
       </c>
@@ -5947,7 +5463,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind | PRICE ALERT</t>
+          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -6007,15 +5523,12 @@
         <v>190</v>
       </c>
       <c r="N72" t="n">
-        <v>88.674797</v>
+        <v>75.68000000000001</v>
       </c>
       <c r="O72">
         <f>M72*N72</f>
         <v/>
       </c>
-      <c r="P72" t="n">
-        <v/>
-      </c>
       <c r="Q72" t="n">
         <v>0</v>
       </c>
@@ -6027,7 +5540,7 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
-          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind | PRICE ALERT</t>
+          <t>PRICE ALERT - Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -6093,9 +5606,6 @@
         <f>M73*N73</f>
         <v/>
       </c>
-      <c r="P73" t="n">
-        <v/>
-      </c>
       <c r="Q73" t="n">
         <v>0</v>
       </c>
@@ -6173,9 +5683,6 @@
         <f>M74*N74</f>
         <v/>
       </c>
-      <c r="P74" t="n">
-        <v/>
-      </c>
       <c r="Q74" t="n">
         <v>0</v>
       </c>
@@ -6253,9 +5760,6 @@
         <f>M75*N75</f>
         <v/>
       </c>
-      <c r="P75" t="n">
-        <v/>
-      </c>
       <c r="Q75" t="n">
         <v>0</v>
       </c>
@@ -6333,9 +5837,6 @@
         <f>M76*N76</f>
         <v/>
       </c>
-      <c r="P76" t="n">
-        <v/>
-      </c>
       <c r="Q76" t="n">
         <v>0</v>
       </c>
@@ -6413,9 +5914,6 @@
         <f>M77*N77</f>
         <v/>
       </c>
-      <c r="P77" t="n">
-        <v/>
-      </c>
       <c r="Q77" t="n">
         <v>0</v>
       </c>
@@ -6493,9 +5991,6 @@
         <f>M78*N78</f>
         <v/>
       </c>
-      <c r="P78" t="n">
-        <v/>
-      </c>
       <c r="Q78" t="n">
         <v>0</v>
       </c>
@@ -6573,9 +6068,6 @@
         <f>M79*N79</f>
         <v/>
       </c>
-      <c r="P79" t="n">
-        <v/>
-      </c>
       <c r="Q79" t="n">
         <v>0</v>
       </c>
@@ -6647,13 +6139,10 @@
         <v>60</v>
       </c>
       <c r="N80" t="n">
-        <v>720.72998</v>
+        <v>613.700012</v>
       </c>
       <c r="O80">
         <f>M80*N80</f>
-        <v/>
-      </c>
-      <c r="P80" t="n">
         <v/>
       </c>
       <c r="Q80" t="n">
@@ -6733,9 +6222,6 @@
         <f>M81*N81</f>
         <v/>
       </c>
-      <c r="P81" t="n">
-        <v/>
-      </c>
       <c r="Q81" t="n">
         <v>0</v>
       </c>
@@ -6807,13 +6293,10 @@
         <v>104.740071</v>
       </c>
       <c r="N82" t="n">
-        <v>127.830002</v>
+        <v>108.870003</v>
       </c>
       <c r="O82">
         <f>M82*N82</f>
-        <v/>
-      </c>
-      <c r="P82" t="n">
         <v/>
       </c>
       <c r="Q82" t="n">
@@ -6893,9 +6376,6 @@
         <f>M83*N83</f>
         <v/>
       </c>
-      <c r="P83" t="n">
-        <v/>
-      </c>
       <c r="Q83" t="n">
         <v>0</v>
       </c>
@@ -6927,7 +6407,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>MSCI World USD (Acc)</t>
+          <t>Core MSCI World USD (Acc)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -6937,7 +6417,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>MWRD</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -6971,9 +6451,6 @@
       </c>
       <c r="O84">
         <f>M84*N84</f>
-        <v/>
-      </c>
-      <c r="P84" t="n">
         <v/>
       </c>
       <c r="Q84" t="n">
@@ -7012,12 +6489,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>IE000BI8OT95</t>
+          <t>IE00B3WJKG14</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>ETF146</t>
+          <t>QDVE.DE</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -7047,13 +6524,10 @@
         <v>220.323194</v>
       </c>
       <c r="N85" t="n">
-        <v>136.712006</v>
+        <v>35.665001</v>
       </c>
       <c r="O85">
         <f>M85*N85</f>
-        <v/>
-      </c>
-      <c r="P85" t="n">
         <v/>
       </c>
       <c r="Q85" t="n">
@@ -7133,9 +6607,6 @@
         <f>M86*N86</f>
         <v/>
       </c>
-      <c r="P86" t="n">
-        <v/>
-      </c>
       <c r="Q86" t="n">
         <v>0</v>
       </c>
@@ -7213,9 +6684,6 @@
         <f>M87*N87</f>
         <v/>
       </c>
-      <c r="P87" t="n">
-        <v/>
-      </c>
       <c r="Q87" t="n">
         <v>0</v>
       </c>
@@ -7293,9 +6761,6 @@
         <f>M88*N88</f>
         <v/>
       </c>
-      <c r="P88" t="n">
-        <v/>
-      </c>
       <c r="Q88" t="n">
         <v>0</v>
       </c>
@@ -7371,9 +6836,6 @@
       </c>
       <c r="O89">
         <f>M89*N89</f>
-        <v/>
-      </c>
-      <c r="P89" t="n">
         <v/>
       </c>
       <c r="Q89" t="n">

</xml_diff>

<commit_message>
chore: checkpoint before dashboard work
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Debug_Timeline" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,8 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="€#,##0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,6 +28,10 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -34,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,15 +49,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="currency" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3048,7 +3060,6 @@
           <t>LU0171310955</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
         <v>4</v>
       </c>
@@ -5292,7 +5303,7 @@
         <v>0.010661</v>
       </c>
       <c r="N69" t="n">
-        <v>104018.22</v>
+        <v>103749.18</v>
       </c>
       <c r="O69">
         <f>M69*N69</f>
@@ -5570,7 +5581,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>MVOL</t>
+          <t>MVOL.MI</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -5600,7 +5611,7 @@
         <v>230</v>
       </c>
       <c r="N73" t="n">
-        <v>62.85</v>
+        <v>62.849998</v>
       </c>
       <c r="O73">
         <f>M73*N73</f>
@@ -5617,7 +5628,7 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t>Aggiornato Manualmente | AssetMind - Da aggiornare manualmente | Aggiornamento manuale richiesto</t>
+          <t>Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6197,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>A111X9</t>
+          <t>EIMI.MI</t>
         </is>
       </c>
       <c r="G81" t="n">
@@ -6216,7 +6227,7 @@
         <v>638.274909</v>
       </c>
       <c r="N81" t="n">
-        <v>37.32</v>
+        <v>37.509998</v>
       </c>
       <c r="O81">
         <f>M81*N81</f>
@@ -6233,7 +6244,7 @@
       </c>
       <c r="T81" t="inlineStr">
         <is>
-          <t>Aggiornato Manualmente | AssetMind - Da aggiornare manualmente | Aggiornamento manuale richiesto</t>
+          <t>Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -6569,11 +6580,6 @@
           <t>LU0171310955</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>MLWTE</t>
-        </is>
-      </c>
       <c r="G86" t="n">
         <v>4</v>
       </c>
@@ -6601,7 +6607,7 @@
         <v>161.21</v>
       </c>
       <c r="N86" t="n">
-        <v>87.13</v>
+        <v>85.550202</v>
       </c>
       <c r="O86">
         <f>M86*N86</f>
@@ -6618,7 +6624,7 @@
       </c>
       <c r="T86" t="inlineStr">
         <is>
-          <t>PIC | Aggiornato Manualmente | AssetMind - Da aggiornare manualmente | Aggiornamento manuale richiesto</t>
+          <t>PIC | Aggiornato Manualmente | UPDATED BY AssetMind</t>
         </is>
       </c>
     </row>
@@ -6851,6 +6857,192 @@
         <is>
           <t>Virgilio | UPDATED BY AssetMind</t>
         </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Criptovalute</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ETF</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fondi di investimento</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>TOTALE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>200204.85498326</v>
+      </c>
+      <c r="D2" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>269192.48966186</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C3" t="n">
+        <v>209206.216685</v>
+      </c>
+      <c r="D3" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E3" t="n">
+        <v>279190.8787446</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-09-04</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C4" t="n">
+        <v>215529.714618344</v>
+      </c>
+      <c r="D4" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>285514.376677944</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C5" t="n">
+        <v>211014.6991230869</v>
+      </c>
+      <c r="D5" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>280999.3611826869</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1073.829225</v>
+      </c>
+      <c r="C6" t="n">
+        <v>269674.234384737</v>
+      </c>
+      <c r="D6" t="n">
+        <v>84384.43033919999</v>
+      </c>
+      <c r="E6" t="n">
+        <v>355132.4939489369</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1119.11523402</v>
+      </c>
+      <c r="C7" t="n">
+        <v>292283.3118653856</v>
+      </c>
+      <c r="D7" t="n">
+        <v>84766.4343524</v>
+      </c>
+      <c r="E7" t="n">
+        <v>378168.8614518056</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1106.07000798</v>
+      </c>
+      <c r="C8" t="n">
+        <v>292607.8108715674</v>
+      </c>
+      <c r="D8" t="n">
+        <v>84451.888846638</v>
+      </c>
+      <c r="E8" t="n">
+        <v>378165.7697261854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use Portfolio button counts as single source of truth for navbar
FINAL FIX: Instead of recalculating counts in navbar, use the exact values
already correctly calculated for the Portfolio buttons.

Changes:
- PortfolioTable._update_button_counts now saves values to attributes
- Added PortfolioTable.get_counts() method to retrieve these values
- main.py._update_navbar_values now calls portfolio_table.get_counts()

This ensures navbar ALWAYS shows the same numbers as Portfolio buttons:
- Record Totali: 88
- Asset Correnti: 43

Single source of truth = Portfolio button calculations.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -6441,7 +6441,7 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" t="n">
         <v>109180</v>
       </c>
       <c r="F2" t="n">
@@ -6456,7 +6456,7 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="J2" t="n">
         <v>109180</v>
       </c>
     </row>
@@ -6475,7 +6475,7 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" t="n">
         <v>234318</v>
       </c>
       <c r="F3" t="n">
@@ -6490,7 +6490,7 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" t="n">
         <v>234318</v>
       </c>
     </row>
@@ -6509,7 +6509,7 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" t="n">
         <v>269592</v>
       </c>
       <c r="F4" t="n">
@@ -6524,7 +6524,7 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" t="n">
         <v>269592</v>
       </c>
     </row>
@@ -6543,7 +6543,7 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" t="n">
         <v>314592</v>
       </c>
       <c r="F5" t="n">
@@ -6558,7 +6558,7 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" t="n">
         <v>314592</v>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" t="n">
         <v>341592</v>
       </c>
       <c r="F6" t="n">
@@ -6592,7 +6592,7 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" t="n">
         <v>341592</v>
       </c>
     </row>
@@ -6611,7 +6611,7 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" t="n">
         <v>612000</v>
       </c>
       <c r="F7" t="n">
@@ -6626,7 +6626,7 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" t="n">
         <v>612000</v>
       </c>
     </row>
@@ -6639,13 +6639,13 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" t="n">
         <v>14391.1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" t="n">
         <v>612000</v>
       </c>
       <c r="F8" t="n">
@@ -6660,7 +6660,7 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" t="n">
         <v>626391.1</v>
       </c>
     </row>
@@ -6673,13 +6673,13 @@
       <c r="B9" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" t="n">
         <v>612000</v>
       </c>
       <c r="F9" t="n">
@@ -6694,7 +6694,7 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" t="n">
         <v>629533.30213</v>
       </c>
     </row>
@@ -6707,13 +6707,13 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" t="n">
         <v>846113</v>
       </c>
       <c r="F10" t="n">
@@ -6728,7 +6728,7 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6741,13 +6741,13 @@
       <c r="B11" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" t="n">
         <v>846113</v>
       </c>
       <c r="F11" t="n">
@@ -6762,7 +6762,7 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6775,13 +6775,13 @@
       <c r="B12" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" t="n">
         <v>1136488</v>
       </c>
       <c r="F12" t="n">
@@ -6796,7 +6796,7 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="5" t="n">
+      <c r="J12" t="n">
         <v>1154021.30213</v>
       </c>
     </row>
@@ -6809,13 +6809,13 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" t="n">
         <v>1838827</v>
       </c>
       <c r="F13" t="n">
@@ -6830,7 +6830,7 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" t="n">
         <v>1856360.30213</v>
       </c>
     </row>
@@ -6843,13 +6843,13 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" t="n">
         <v>1838827</v>
       </c>
       <c r="F14" t="n">
@@ -6864,7 +6864,7 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" t="n">
         <v>1862369.308154</v>
       </c>
     </row>
@@ -6877,19 +6877,19 @@
       <c r="B15" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" t="n">
         <v>1838827</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" t="n">
         <v>163008</v>
       </c>
       <c r="H15" t="n">
@@ -6898,7 +6898,7 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" t="n">
         <v>2025377.308154</v>
       </c>
     </row>
@@ -6911,19 +6911,19 @@
       <c r="B16" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" t="n">
         <v>1838827</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" t="n">
         <v>391000</v>
       </c>
       <c r="H16" t="n">
@@ -6932,7 +6932,7 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" t="n">
         <v>2253369.308154</v>
       </c>
     </row>
@@ -6945,28 +6945,28 @@
       <c r="B17" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" t="n">
         <v>155263.63205</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" t="n">
         <v>1838827</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" t="n">
         <v>391000</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="H17" t="n">
         <v>44998.8521765</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" s="5" t="n">
+      <c r="J17" t="n">
         <v>2436098.4902505</v>
       </c>
     </row>
@@ -6979,28 +6979,28 @@
       <c r="B18" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" t="n">
         <v>1838827</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" t="n">
         <v>391000</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I18" s="5" t="n">
+      <c r="I18" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="J18" t="n">
         <v>2583792.5511051</v>
       </c>
     </row>
@@ -7013,28 +7013,28 @@
       <c r="B19" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" t="n">
         <v>1846827</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" t="n">
         <v>391000</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" t="n">
         <v>2591792.5511051</v>
       </c>
     </row>
@@ -7047,28 +7047,28 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" t="n">
         <v>1846827</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" t="n">
         <v>391000</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" t="n">
         <v>2602899.68403836</v>
       </c>
     </row>
@@ -7081,28 +7081,28 @@
       <c r="B21" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" t="n">
         <v>1846827</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" t="n">
         <v>391000</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="H21" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I21" s="5" t="n">
+      <c r="I21" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" t="n">
         <v>2621762.38356186</v>
       </c>
     </row>
@@ -7115,28 +7115,28 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" t="n">
         <v>1846827</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H22" s="5" t="n">
+      <c r="H22" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I22" s="5" t="n">
+      <c r="I22" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J22" s="5" t="n">
+      <c r="J22" t="n">
         <v>2636253.103561861</v>
       </c>
     </row>
@@ -7146,31 +7146,31 @@
           <t>2025-08-26</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B23" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" t="n">
         <v>1846827</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="G23" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H23" s="5" t="n">
+      <c r="H23" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I23" s="5" t="n">
+      <c r="I23" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J23" s="5" t="n">
+      <c r="J23" t="n">
         <v>2646251.4926446</v>
       </c>
     </row>
@@ -7180,31 +7180,31 @@
           <t>2025-09-03</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n">
+      <c r="B24" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" t="n">
         <v>2051827</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="J24" t="n">
         <v>2851251.4926446</v>
       </c>
     </row>
@@ -7214,31 +7214,31 @@
           <t>2025-09-04</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B25" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" t="n">
         <v>2270000</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="G25" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" t="n">
         <v>3075747.990577944</v>
       </c>
     </row>
@@ -7248,31 +7248,31 @@
           <t>2025-09-08</t>
         </is>
       </c>
-      <c r="B26" s="5" t="n">
+      <c r="B26" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" t="n">
         <v>2270000</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G26" s="5" t="n">
+      <c r="G26" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H26" s="5" t="n">
+      <c r="H26" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I26" s="5" t="n">
+      <c r="I26" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J26" s="5" t="n">
+      <c r="J26" t="n">
         <v>3092047.550577944</v>
       </c>
     </row>
@@ -7282,31 +7282,31 @@
           <t>2025-10-01</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B27" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" t="n">
         <v>211014.6991230869</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="D27" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" t="n">
         <v>2270000</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="G27" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H27" s="5" t="n">
+      <c r="H27" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I27" s="5" t="n">
+      <c r="I27" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J27" s="5" t="n">
+      <c r="J27" t="n">
         <v>3087532.535082687</v>
       </c>
     </row>
@@ -7316,31 +7316,31 @@
           <t>2025-10-02</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" t="n">
         <v>1073.829225</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" t="n">
         <v>269674.234384737</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" t="n">
         <v>84384.43033919999</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" t="n">
         <v>2270000</v>
       </c>
-      <c r="F28" s="5" t="n">
+      <c r="F28" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G28" s="5" t="n">
+      <c r="G28" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H28" s="5" t="n">
+      <c r="H28" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
-      <c r="J28" s="5" t="n">
+      <c r="J28" t="n">
         <v>3159575.785648937</v>
       </c>
     </row>
@@ -7350,31 +7350,31 @@
           <t>2025-10-03</t>
         </is>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B29" t="n">
         <v>1119.11523402</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" t="n">
         <v>292283.3118653856</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" t="n">
         <v>84766.4343524</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" t="n">
         <v>2270000</v>
       </c>
-      <c r="F29" s="5" t="n">
+      <c r="F29" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G29" s="5" t="n">
+      <c r="G29" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" t="n">
         <v>3187769.273151806</v>
       </c>
     </row>
@@ -7384,31 +7384,31 @@
           <t>2025-10-05</t>
         </is>
       </c>
-      <c r="B30" s="5" t="n">
+      <c r="B30" t="n">
         <v>1106.07000798</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" t="n">
         <v>292607.8108715674</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" t="n">
         <v>84451.888846638</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" t="n">
         <v>2270000</v>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G30" s="5" t="n">
+      <c r="G30" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" t="n">
         <v>2100.273</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" t="n">
         <v>3189866.454426186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add active selection indicator to RoadMap header
Shows current filter state next to "RoadMap AssetMind" title:
- "Patrimonio Complessivo" when no filters active
- Filter details when filters applied (e.g., "Categoria: ETF | Rischio: 3")
- Compact format: shows first 2 values, then "+N" if more

Matches behavior of Grafici and Export screens for consistency.

Changes:
- Added filter_label to RoadMap header
- Pass filter_state from main.py to RoadMap.refresh()
- Format filters in _update_filter_label() method
- Uses FieldMapping for display names

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -6354,7 +6354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6365,13 +6365,6 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="17" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6382,45 +6375,10 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>Criptovalute</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>ETF</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>Fondi di investimento</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>Immobiliare</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>Liquidità</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>Oggetti</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>PAC</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>Titoli di stato</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>TOTALE</t>
         </is>
@@ -6429,987 +6387,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1989-01-16</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>101288.92992</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>109180</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>109180</v>
+        <v>101288.92992</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1997-01-17</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>95856.314652</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>234318</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>234318</v>
+        <v>95856.314652</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1997-12-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>143818.614652</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>269592</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>269592</v>
+        <v>143818.614652</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2004-05-21</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>144533.019342</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>314592</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>314592</v>
+        <v>144533.019342</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2006-05-22</t>
+          <t>2025-10-05</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>144527.007747</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>341592</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>341592</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2008-05-22</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>612000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>612000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2012-11-30</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>14391.1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>612000</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>626391.1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2014-05-30</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>612000</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>629533.30213</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2015-04-08</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>846113</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>863646.30213</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2015-05-22</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>846113</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>863646.30213</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2015-05-27</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1136488</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1154021.30213</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2015-08-04</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1856360.30213</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2019-07-16</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D14" t="n">
-        <v>6009.006024</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>1862369.308154</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2020-02-11</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D15" t="n">
-        <v>6009.006024</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>163008</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>2025377.308154</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2020-11-02</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>17533.30213</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6009.006024</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>2253369.308154</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-11-13</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>155263.63205</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6009.006024</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H17" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>2436098.4902505</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-11-14</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>189097.72205</v>
-      </c>
-      <c r="D18" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1838827</v>
-      </c>
-      <c r="F18" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G18" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H18" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="I18" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J18" t="n">
-        <v>2583792.5511051</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-03-09</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>189097.72205</v>
-      </c>
-      <c r="D19" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1846827</v>
-      </c>
-      <c r="F19" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G19" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H19" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="I19" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J19" t="n">
-        <v>2591792.5511051</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>200204.85498326</v>
-      </c>
-      <c r="D20" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1846827</v>
-      </c>
-      <c r="F20" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G20" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H20" t="n">
-        <v>44998.8521765</v>
-      </c>
-      <c r="I20" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J20" t="n">
-        <v>2602899.68403836</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2025-05-19</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>200204.85498326</v>
-      </c>
-      <c r="D21" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1846827</v>
-      </c>
-      <c r="F21" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G21" t="n">
-        <v>391000</v>
-      </c>
-      <c r="H21" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I21" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J21" t="n">
-        <v>2621762.38356186</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2025-07-31</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>200204.85498326</v>
-      </c>
-      <c r="D22" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1846827</v>
-      </c>
-      <c r="F22" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G22" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H22" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I22" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J22" t="n">
-        <v>2636253.103561861</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2025-08-26</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>997.027381</v>
-      </c>
-      <c r="C23" t="n">
-        <v>209206.216685</v>
-      </c>
-      <c r="D23" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1846827</v>
-      </c>
-      <c r="F23" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G23" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H23" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I23" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J23" t="n">
-        <v>2646251.4926446</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2025-09-03</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>997.027381</v>
-      </c>
-      <c r="C24" t="n">
-        <v>209206.216685</v>
-      </c>
-      <c r="D24" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2051827</v>
-      </c>
-      <c r="F24" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G24" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H24" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I24" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J24" t="n">
-        <v>2851251.4926446</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2025-09-04</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>997.027381</v>
-      </c>
-      <c r="C25" t="n">
-        <v>215529.714618344</v>
-      </c>
-      <c r="D25" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E25" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F25" t="n">
-        <v>48791.46</v>
-      </c>
-      <c r="G25" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H25" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I25" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J25" t="n">
-        <v>3075747.990577944</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2025-09-08</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>997.027381</v>
-      </c>
-      <c r="C26" t="n">
-        <v>215529.714618344</v>
-      </c>
-      <c r="D26" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E26" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F26" t="n">
-        <v>65091.02</v>
-      </c>
-      <c r="G26" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H26" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I26" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J26" t="n">
-        <v>3092047.550577944</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2025-10-01</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>997.027381</v>
-      </c>
-      <c r="C27" t="n">
-        <v>211014.6991230869</v>
-      </c>
-      <c r="D27" t="n">
-        <v>68987.63467860001</v>
-      </c>
-      <c r="E27" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F27" t="n">
-        <v>65091.02</v>
-      </c>
-      <c r="G27" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H27" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I27" t="n">
-        <v>2089.8822</v>
-      </c>
-      <c r="J27" t="n">
-        <v>3087532.535082687</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2025-10-02</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1073.829225</v>
-      </c>
-      <c r="C28" t="n">
-        <v>269674.234384737</v>
-      </c>
-      <c r="D28" t="n">
-        <v>84384.43033919999</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F28" t="n">
-        <v>65091.02</v>
-      </c>
-      <c r="G28" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H28" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>3159575.785648937</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2025-10-03</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1119.11523402</v>
-      </c>
-      <c r="C29" t="n">
-        <v>292283.3118653856</v>
-      </c>
-      <c r="D29" t="n">
-        <v>84766.4343524</v>
-      </c>
-      <c r="E29" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F29" t="n">
-        <v>70248.14</v>
-      </c>
-      <c r="G29" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H29" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" t="n">
-        <v>3187769.273151806</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-10-05</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1106.07000798</v>
-      </c>
-      <c r="C30" t="n">
-        <v>292607.8108715674</v>
-      </c>
-      <c r="D30" t="n">
-        <v>84451.888846638</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2270000</v>
-      </c>
-      <c r="F30" t="n">
-        <v>70248.14</v>
-      </c>
-      <c r="G30" t="n">
-        <v>405490.72</v>
-      </c>
-      <c r="H30" t="n">
-        <v>63861.5517</v>
-      </c>
-      <c r="I30" t="n">
-        <v>2100.273</v>
-      </c>
-      <c r="J30" t="n">
-        <v>3189866.454426186</v>
+        <v>144527.007747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Standardize filter display across all screens
Changes:
- Removed "+N" compact format from RoadMap (now shows all values)
- Added "Patrimonio Complessivo" to Grafici when no filters active
- Added "Patrimonio Complessivo" to Export when no filters active

Now all three screens (RoadMap, Grafici, Export) behave consistently:
- Show "Patrimonio Complessivo" when viewing all assets
- Show complete filter details when filters are applied
- Use same format: "Campo: val1, val2, val3"

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -6354,7 +6354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6365,6 +6365,13 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="17" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6375,10 +6382,45 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
+          <t>Criptovalute</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
           <t>ETF</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Fondi di investimento</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Immobiliare</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Liquidità</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Oggetti</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>PAC</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Titoli di stato</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>TOTALE</t>
         </is>
@@ -6387,66 +6429,987 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>1989-01-16</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101288.92992</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>101288.92992</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>109180</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>109180</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>1997-01-17</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>95856.314652</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>95856.314652</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>234318</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>234318</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>1997-12-01</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>143818.614652</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>143818.614652</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>269592</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>269592</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2004-05-21</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>144533.019342</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>144533.019342</v>
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>314592</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>314592</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2006-05-22</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>341592</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>341592</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2008-05-22</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>612000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>612000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2012-11-30</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14391.1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>612000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>626391.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2014-05-30</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>612000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>629533.30213</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2015-04-08</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>846113</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>863646.30213</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2015-05-22</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>846113</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>863646.30213</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2015-05-27</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1136488</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1154021.30213</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2015-08-04</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1856360.30213</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2019-07-16</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6009.006024</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1862369.308154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2020-02-11</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6009.006024</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>163008</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2025377.308154</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2020-11-02</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>17533.30213</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6009.006024</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2253369.308154</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>155263.63205</v>
+      </c>
+      <c r="D17" t="n">
+        <v>6009.006024</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H17" t="n">
+        <v>44998.8521765</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2436098.4902505</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-11-14</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>189097.72205</v>
+      </c>
+      <c r="D18" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1838827</v>
+      </c>
+      <c r="F18" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G18" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H18" t="n">
+        <v>44998.8521765</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2583792.5511051</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-09</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>189097.72205</v>
+      </c>
+      <c r="D19" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1846827</v>
+      </c>
+      <c r="F19" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G19" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>44998.8521765</v>
+      </c>
+      <c r="I19" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2591792.5511051</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>200204.85498326</v>
+      </c>
+      <c r="D20" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1846827</v>
+      </c>
+      <c r="F20" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G20" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>44998.8521765</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2602899.68403836</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>200204.85498326</v>
+      </c>
+      <c r="D21" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1846827</v>
+      </c>
+      <c r="F21" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G21" t="n">
+        <v>391000</v>
+      </c>
+      <c r="H21" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2621762.38356186</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-07-31</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>200204.85498326</v>
+      </c>
+      <c r="D22" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1846827</v>
+      </c>
+      <c r="F22" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G22" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H22" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2636253.103561861</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C23" t="n">
+        <v>209206.216685</v>
+      </c>
+      <c r="D23" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1846827</v>
+      </c>
+      <c r="F23" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G23" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H23" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2646251.4926446</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C24" t="n">
+        <v>209206.216685</v>
+      </c>
+      <c r="D24" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2051827</v>
+      </c>
+      <c r="F24" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G24" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H24" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2851251.4926446</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-09-04</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C25" t="n">
+        <v>215529.714618344</v>
+      </c>
+      <c r="D25" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F25" t="n">
+        <v>48791.46</v>
+      </c>
+      <c r="G25" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H25" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J25" t="n">
+        <v>3075747.990577944</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C26" t="n">
+        <v>215529.714618344</v>
+      </c>
+      <c r="D26" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F26" t="n">
+        <v>65091.02</v>
+      </c>
+      <c r="G26" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H26" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3092047.550577944</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>997.027381</v>
+      </c>
+      <c r="C27" t="n">
+        <v>211014.6991230869</v>
+      </c>
+      <c r="D27" t="n">
+        <v>68987.63467860001</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>65091.02</v>
+      </c>
+      <c r="G27" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H27" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I27" t="n">
+        <v>2089.8822</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3087532.535082687</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1073.829225</v>
+      </c>
+      <c r="C28" t="n">
+        <v>269674.234384737</v>
+      </c>
+      <c r="D28" t="n">
+        <v>84384.43033919999</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F28" t="n">
+        <v>65091.02</v>
+      </c>
+      <c r="G28" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H28" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3159575.785648937</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1119.11523402</v>
+      </c>
+      <c r="C29" t="n">
+        <v>292283.3118653856</v>
+      </c>
+      <c r="D29" t="n">
+        <v>84766.4343524</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F29" t="n">
+        <v>70248.14</v>
+      </c>
+      <c r="G29" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H29" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3187769.273151806</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>2025-10-05</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>144527.007747</v>
-      </c>
-      <c r="C6" t="n">
-        <v>144527.007747</v>
+      <c r="B30" t="n">
+        <v>1106.07000798</v>
+      </c>
+      <c r="C30" t="n">
+        <v>292607.8108715674</v>
+      </c>
+      <c r="D30" t="n">
+        <v>84451.888846638</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2270000</v>
+      </c>
+      <c r="F30" t="n">
+        <v>70248.14</v>
+      </c>
+      <c r="G30" t="n">
+        <v>405490.72</v>
+      </c>
+      <c r="H30" t="n">
+        <v>63861.5517</v>
+      </c>
+      <c r="I30" t="n">
+        <v>2100.273</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3189866.454426186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve PDF export with A3 landscape table and Portfolio column alignment
- Changed detail asset table from A4 to A3 landscape (16.54 x 11.69 inches)
- Match table columns exactly with Portfolio table in same order
- Add all Portfolio fields: id, category, position, asset_name, isin, ticker, risk_level, dates, amounts, prices, accumulation, income, note
- Implement word wrap for long text fields (asset_name: 40 chars, note: 50 chars)
- Improve table formatting: left-aligned text, alternating row colors, blue header
- Increase DPI to 150 for better readability
- Reduce rows per page to 22 to accommodate wrapped text
- Use FieldMapping for proper column headers

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -6441,7 +6441,7 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="5" t="n">
         <v>109180</v>
       </c>
       <c r="F2" t="n">
@@ -6456,7 +6456,7 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" s="5" t="n">
         <v>109180</v>
       </c>
     </row>
@@ -6475,7 +6475,7 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="5" t="n">
         <v>234318</v>
       </c>
       <c r="F3" t="n">
@@ -6490,7 +6490,7 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="5" t="n">
         <v>234318</v>
       </c>
     </row>
@@ -6509,7 +6509,7 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="5" t="n">
         <v>269592</v>
       </c>
       <c r="F4" t="n">
@@ -6524,7 +6524,7 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="5" t="n">
         <v>269592</v>
       </c>
     </row>
@@ -6543,7 +6543,7 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="5" t="n">
         <v>314592</v>
       </c>
       <c r="F5" t="n">
@@ -6558,7 +6558,7 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="5" t="n">
         <v>314592</v>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="5" t="n">
         <v>341592</v>
       </c>
       <c r="F6" t="n">
@@ -6592,7 +6592,7 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="5" t="n">
         <v>341592</v>
       </c>
     </row>
@@ -6611,7 +6611,7 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="5" t="n">
         <v>612000</v>
       </c>
       <c r="F7" t="n">
@@ -6626,7 +6626,7 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="5" t="n">
         <v>612000</v>
       </c>
     </row>
@@ -6639,13 +6639,13 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="5" t="n">
         <v>14391.1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="5" t="n">
         <v>612000</v>
       </c>
       <c r="F8" t="n">
@@ -6660,7 +6660,7 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="5" t="n">
         <v>626391.1</v>
       </c>
     </row>
@@ -6673,13 +6673,13 @@
       <c r="B9" t="n">
         <v>0</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="5" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="5" t="n">
         <v>612000</v>
       </c>
       <c r="F9" t="n">
@@ -6694,7 +6694,7 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="5" t="n">
         <v>629533.30213</v>
       </c>
     </row>
@@ -6707,13 +6707,13 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="5" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="5" t="n">
         <v>846113</v>
       </c>
       <c r="F10" t="n">
@@ -6728,7 +6728,7 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="5" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6741,13 +6741,13 @@
       <c r="B11" t="n">
         <v>0</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="5" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="5" t="n">
         <v>846113</v>
       </c>
       <c r="F11" t="n">
@@ -6762,7 +6762,7 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="5" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6775,13 +6775,13 @@
       <c r="B12" t="n">
         <v>0</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="5" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="5" t="n">
         <v>1136488</v>
       </c>
       <c r="F12" t="n">
@@ -6796,7 +6796,7 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="5" t="n">
         <v>1154021.30213</v>
       </c>
     </row>
@@ -6809,13 +6809,13 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="5" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="5" t="n">
         <v>1838827</v>
       </c>
       <c r="F13" t="n">
@@ -6830,7 +6830,7 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="5" t="n">
         <v>1856360.30213</v>
       </c>
     </row>
@@ -6843,13 +6843,13 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="5" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="5" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="5" t="n">
         <v>1838827</v>
       </c>
       <c r="F14" t="n">
@@ -6864,7 +6864,7 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="5" t="n">
         <v>1862369.308154</v>
       </c>
     </row>
@@ -6877,19 +6877,19 @@
       <c r="B15" t="n">
         <v>0</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="5" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="5" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="5" t="n">
         <v>1838827</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="5" t="n">
         <v>163008</v>
       </c>
       <c r="H15" t="n">
@@ -6898,7 +6898,7 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="5" t="n">
         <v>2025377.308154</v>
       </c>
     </row>
@@ -6911,19 +6911,19 @@
       <c r="B16" t="n">
         <v>0</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="5" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="5" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="5" t="n">
         <v>1838827</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" s="5" t="n">
         <v>391000</v>
       </c>
       <c r="H16" t="n">
@@ -6932,7 +6932,7 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" s="5" t="n">
         <v>2253369.308154</v>
       </c>
     </row>
@@ -6945,28 +6945,28 @@
       <c r="B17" t="n">
         <v>0</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="5" t="n">
         <v>155263.63205</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="5" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="5" t="n">
         <v>1838827</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" s="5" t="n">
         <v>391000</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="5" t="n">
         <v>44998.8521765</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" s="5" t="n">
         <v>2436098.4902505</v>
       </c>
     </row>
@@ -6979,28 +6979,28 @@
       <c r="B18" t="n">
         <v>0</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="5" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="5" t="n">
         <v>1838827</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="5" t="n">
         <v>391000</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="5" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" s="5" t="n">
         <v>2583792.5511051</v>
       </c>
     </row>
@@ -7013,28 +7013,28 @@
       <c r="B19" t="n">
         <v>0</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="5" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="5" t="n">
         <v>1846827</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="5" t="n">
         <v>391000</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="5" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="5" t="n">
         <v>2591792.5511051</v>
       </c>
     </row>
@@ -7047,28 +7047,28 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="5" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="5" t="n">
         <v>1846827</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="5" t="n">
         <v>391000</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="5" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" s="5" t="n">
         <v>2602899.68403836</v>
       </c>
     </row>
@@ -7081,28 +7081,28 @@
       <c r="B21" t="n">
         <v>0</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="5" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="5" t="n">
         <v>1846827</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="5" t="n">
         <v>391000</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="5" t="n">
         <v>2621762.38356186</v>
       </c>
     </row>
@@ -7115,28 +7115,28 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="5" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="5" t="n">
         <v>1846827</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="5" t="n">
         <v>2636253.103561861</v>
       </c>
     </row>
@@ -7146,31 +7146,31 @@
           <t>2025-08-26</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="5" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="5" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="5" t="n">
         <v>1846827</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J23" s="5" t="n">
         <v>2646251.4926446</v>
       </c>
     </row>
@@ -7180,31 +7180,31 @@
           <t>2025-09-03</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="5" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="5" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="5" t="n">
         <v>2051827</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24" s="5" t="n">
         <v>2851251.4926446</v>
       </c>
     </row>
@@ -7214,31 +7214,31 @@
           <t>2025-09-04</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="5" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="5" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" s="5" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25" s="5" t="n">
         <v>3075747.990577944</v>
       </c>
     </row>
@@ -7248,31 +7248,31 @@
           <t>2025-09-08</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="5" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="5" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26" s="5" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" s="5" t="n">
         <v>3092047.550577944</v>
       </c>
     </row>
@@ -7282,31 +7282,31 @@
           <t>2025-10-01</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="5" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="5" t="n">
         <v>211014.6991230869</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="5" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27" s="5" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" s="5" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" s="5" t="n">
         <v>3087532.535082687</v>
       </c>
     </row>
@@ -7316,31 +7316,31 @@
           <t>2025-10-02</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" s="5" t="n">
         <v>1073.829225</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="5" t="n">
         <v>269674.234384737</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="5" t="n">
         <v>84384.43033919999</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28" s="5" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28" s="5" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J28" s="5" t="n">
         <v>3159575.785648937</v>
       </c>
     </row>
@@ -7350,31 +7350,31 @@
           <t>2025-10-03</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" s="5" t="n">
         <v>1119.11523402</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="5" t="n">
         <v>292283.3118653856</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="5" t="n">
         <v>84766.4343524</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29" s="5" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G29" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29" s="5" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" s="5" t="n">
         <v>3187769.273151806</v>
       </c>
     </row>
@@ -7384,31 +7384,31 @@
           <t>2025-10-05</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B30" s="5" t="n">
         <v>1106.07000798</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="5" t="n">
         <v>292607.8108715674</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" s="5" t="n">
         <v>84451.888846638</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" s="5" t="n">
         <v>2270000</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30" s="5" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" s="5" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30" s="5" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" s="5" t="n">
         <v>2100.273</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" s="5" t="n">
         <v>3189866.454426186</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimize PDF table layout with minimal margins and column-specific widths
- Reduce page margins to 0.5cm for maximum table space
- Implement variable column widths: minimal for IDs/dates/numbers, generous for asset names and notes
- Add proper text wrapping using textwrap.fill() for long fields
- Improve formatting: reduce decimal places for amounts (,.2f instead of ,.4f)
- Use fig.add_axes for precise margin control
- Increase cell height to 0.045 for better wrapped text display
- Apply bbox_inches='tight' for optimal PDF space usage

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/portfolio_data.xlsx
+++ b/portfolio_data.xlsx
@@ -6441,7 +6441,7 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" t="n">
         <v>109180</v>
       </c>
       <c r="F2" t="n">
@@ -6456,7 +6456,7 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="J2" t="n">
         <v>109180</v>
       </c>
     </row>
@@ -6475,7 +6475,7 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" t="n">
         <v>234318</v>
       </c>
       <c r="F3" t="n">
@@ -6490,7 +6490,7 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" t="n">
         <v>234318</v>
       </c>
     </row>
@@ -6509,7 +6509,7 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" t="n">
         <v>269592</v>
       </c>
       <c r="F4" t="n">
@@ -6524,7 +6524,7 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" t="n">
         <v>269592</v>
       </c>
     </row>
@@ -6543,7 +6543,7 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" t="n">
         <v>314592</v>
       </c>
       <c r="F5" t="n">
@@ -6558,7 +6558,7 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" t="n">
         <v>314592</v>
       </c>
     </row>
@@ -6577,7 +6577,7 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" t="n">
         <v>341592</v>
       </c>
       <c r="F6" t="n">
@@ -6592,7 +6592,7 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" t="n">
         <v>341592</v>
       </c>
     </row>
@@ -6611,7 +6611,7 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" t="n">
         <v>612000</v>
       </c>
       <c r="F7" t="n">
@@ -6626,7 +6626,7 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" t="n">
         <v>612000</v>
       </c>
     </row>
@@ -6639,13 +6639,13 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" t="n">
         <v>14391.1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" t="n">
         <v>612000</v>
       </c>
       <c r="F8" t="n">
@@ -6660,7 +6660,7 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" t="n">
         <v>626391.1</v>
       </c>
     </row>
@@ -6673,13 +6673,13 @@
       <c r="B9" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" t="n">
         <v>612000</v>
       </c>
       <c r="F9" t="n">
@@ -6694,7 +6694,7 @@
       <c r="I9" t="n">
         <v>0</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" t="n">
         <v>629533.30213</v>
       </c>
     </row>
@@ -6707,13 +6707,13 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" t="n">
         <v>846113</v>
       </c>
       <c r="F10" t="n">
@@ -6728,7 +6728,7 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6741,13 +6741,13 @@
       <c r="B11" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" t="n">
         <v>846113</v>
       </c>
       <c r="F11" t="n">
@@ -6762,7 +6762,7 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" t="n">
         <v>863646.30213</v>
       </c>
     </row>
@@ -6775,13 +6775,13 @@
       <c r="B12" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" t="n">
         <v>1136488</v>
       </c>
       <c r="F12" t="n">
@@ -6796,7 +6796,7 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" s="5" t="n">
+      <c r="J12" t="n">
         <v>1154021.30213</v>
       </c>
     </row>
@@ -6809,13 +6809,13 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" t="n">
         <v>17533.30213</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" t="n">
         <v>1838827</v>
       </c>
       <c r="F13" t="n">
@@ -6830,7 +6830,7 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" t="n">
         <v>1856360.30213</v>
       </c>
     </row>
@@ -6843,13 +6843,13 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" t="n">
         <v>1838827</v>
       </c>
       <c r="F14" t="n">
@@ -6864,7 +6864,7 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" t="n">
         <v>1862369.308154</v>
       </c>
     </row>
@@ -6877,19 +6877,19 @@
       <c r="B15" t="n">
         <v>0</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" t="n">
         <v>1838827</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" t="n">
         <v>163008</v>
       </c>
       <c r="H15" t="n">
@@ -6898,7 +6898,7 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" t="n">
         <v>2025377.308154</v>
       </c>
     </row>
@@ -6911,19 +6911,19 @@
       <c r="B16" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" t="n">
         <v>17533.30213</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" t="n">
         <v>1838827</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" t="n">
         <v>391000</v>
       </c>
       <c r="H16" t="n">
@@ -6932,7 +6932,7 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" t="n">
         <v>2253369.308154</v>
       </c>
     </row>
@@ -6945,28 +6945,28 @@
       <c r="B17" t="n">
         <v>0</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" t="n">
         <v>155263.63205</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" t="n">
         <v>6009.006024</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" t="n">
         <v>1838827</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" t="n">
         <v>391000</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="H17" t="n">
         <v>44998.8521765</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" s="5" t="n">
+      <c r="J17" t="n">
         <v>2436098.4902505</v>
       </c>
     </row>
@@ -6979,28 +6979,28 @@
       <c r="B18" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" t="n">
         <v>1838827</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" t="n">
         <v>391000</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I18" s="5" t="n">
+      <c r="I18" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="J18" t="n">
         <v>2583792.5511051</v>
       </c>
     </row>
@@ -7013,28 +7013,28 @@
       <c r="B19" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" t="n">
         <v>189097.72205</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" t="n">
         <v>1846827</v>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" t="n">
         <v>391000</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" t="n">
         <v>2591792.5511051</v>
       </c>
     </row>
@@ -7047,28 +7047,28 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" t="n">
         <v>1846827</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" t="n">
         <v>391000</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="H20" t="n">
         <v>44998.8521765</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" t="n">
         <v>2602899.68403836</v>
       </c>
     </row>
@@ -7081,28 +7081,28 @@
       <c r="B21" t="n">
         <v>0</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" t="n">
         <v>1846827</v>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" t="n">
         <v>391000</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="H21" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I21" s="5" t="n">
+      <c r="I21" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" t="n">
         <v>2621762.38356186</v>
       </c>
     </row>
@@ -7115,28 +7115,28 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" t="n">
         <v>200204.85498326</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" t="n">
         <v>1846827</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H22" s="5" t="n">
+      <c r="H22" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I22" s="5" t="n">
+      <c r="I22" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J22" s="5" t="n">
+      <c r="J22" t="n">
         <v>2636253.103561861</v>
       </c>
     </row>
@@ -7146,31 +7146,31 @@
           <t>2025-08-26</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B23" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" t="n">
         <v>1846827</v>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="G23" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H23" s="5" t="n">
+      <c r="H23" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I23" s="5" t="n">
+      <c r="I23" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J23" s="5" t="n">
+      <c r="J23" t="n">
         <v>2646251.4926446</v>
       </c>
     </row>
@@ -7180,31 +7180,31 @@
           <t>2025-09-03</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n">
+      <c r="B24" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" t="n">
         <v>209206.216685</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" t="n">
         <v>2051827</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="H24" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="J24" t="n">
         <v>2851251.4926446</v>
       </c>
     </row>
@@ -7214,31 +7214,31 @@
           <t>2025-09-04</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B25" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" t="n">
         <v>2270000</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" t="n">
         <v>48791.46</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="G25" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="H25" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" t="n">
         <v>3075747.990577944</v>
       </c>
     </row>
@@ -7248,31 +7248,31 @@
           <t>2025-09-08</t>
         </is>
       </c>
-      <c r="B26" s="5" t="n">
+      <c r="B26" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" t="n">
         <v>215529.714618344</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" t="n">
         <v>2270000</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G26" s="5" t="n">
+      <c r="G26" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H26" s="5" t="n">
+      <c r="H26" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I26" s="5" t="n">
+      <c r="I26" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J26" s="5" t="n">
+      <c r="J26" t="n">
         <v>3092047.550577944</v>
       </c>
     </row>
@@ -7282,31 +7282,31 @@
           <t>2025-10-01</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B27" t="n">
         <v>997.027381</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" t="n">
         <v>211014.6991230869</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="D27" t="n">
         <v>68987.63467860001</v>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" t="n">
         <v>2270000</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="G27" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H27" s="5" t="n">
+      <c r="H27" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I27" s="5" t="n">
+      <c r="I27" t="n">
         <v>2089.8822</v>
       </c>
-      <c r="J27" s="5" t="n">
+      <c r="J27" t="n">
         <v>3087532.535082687</v>
       </c>
     </row>
@@ -7316,31 +7316,31 @@
           <t>2025-10-02</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" t="n">
         <v>1073.829225</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" t="n">
         <v>269674.234384737</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" t="n">
         <v>84384.43033919999</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" t="n">
         <v>2270000</v>
       </c>
-      <c r="F28" s="5" t="n">
+      <c r="F28" t="n">
         <v>65091.02</v>
       </c>
-      <c r="G28" s="5" t="n">
+      <c r="G28" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H28" s="5" t="n">
+      <c r="H28" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
-      <c r="J28" s="5" t="n">
+      <c r="J28" t="n">
         <v>3159575.785648937</v>
       </c>
     </row>
@@ -7350,31 +7350,31 @@
           <t>2025-10-03</t>
         </is>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B29" t="n">
         <v>1119.11523402</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" t="n">
         <v>292283.3118653856</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" t="n">
         <v>84766.4343524</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" t="n">
         <v>2270000</v>
       </c>
-      <c r="F29" s="5" t="n">
+      <c r="F29" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G29" s="5" t="n">
+      <c r="G29" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" t="n">
         <v>63861.5517</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" t="n">
         <v>3187769.273151806</v>
       </c>
     </row>
@@ -7384,31 +7384,31 @@
           <t>2025-10-05</t>
         </is>
       </c>
-      <c r="B30" s="5" t="n">
+      <c r="B30" t="n">
         <v>1106.07000798</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" t="n">
         <v>292607.8108715674</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" t="n">
         <v>84451.888846638</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" t="n">
         <v>2270000</v>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" t="n">
         <v>70248.14</v>
       </c>
-      <c r="G30" s="5" t="n">
+      <c r="G30" t="n">
         <v>405490.72</v>
       </c>
-      <c r="H30" s="5" t="n">
+      <c r="H30" t="n">
         <v>63861.5517</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" t="n">
         <v>2100.273</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" t="n">
         <v>3189866.454426186</v>
       </c>
     </row>

</xml_diff>